<commit_message>
modify : cross 이슈 해결
</commit_message>
<xml_diff>
--- a/vulnerability-scanner/output/vulnerability-dashboard.xlsx
+++ b/vulnerability-scanner/output/vulnerability-dashboard.xlsx
@@ -22,7 +22,7 @@
     <t>Scan Date:</t>
   </si>
   <si>
-    <t>2025. 12. 8. 오후 4:42:40</t>
+    <t>2025. 12. 9. 오전 11:09:00</t>
   </si>
   <si>
     <t>Scanner Version:</t>
@@ -130,16 +130,22 @@
     <t>tour-api</t>
   </si>
   <si>
+    <t>/Users/milk/workspace/boilerplate-maven/step-hts-server</t>
+  </si>
+  <si>
+    <t>step-hts-server</t>
+  </si>
+  <si>
     <t>/Users/milk/workspace/boilerplate-maven/scm-api</t>
   </si>
   <si>
     <t>scm-api</t>
   </si>
   <si>
-    <t>/Users/milk/workspace/boilerplate-maven/step-hts-server</t>
-  </si>
-  <si>
-    <t>step-hts-server</t>
+    <t>/Users/milk/workspace/boilerplate-maven/partner-gateway</t>
+  </si>
+  <si>
+    <t>partner-gateway</t>
   </si>
   <si>
     <t>/Users/milk/workspace/boilerplate-maven/order</t>
@@ -166,69 +172,63 @@
     <t>gateway-domain</t>
   </si>
   <si>
-    <t>/Users/milk/workspace/boilerplate-maven/partner-gateway</t>
-  </si>
-  <si>
-    <t>partner-gateway</t>
-  </si>
-  <si>
     <t>/Users/milk/workspace/boilerplate-maven/channel-gateway</t>
   </si>
   <si>
     <t>channel-gateway</t>
   </si>
   <si>
+    <t>/Users/milk/workspace/boilerplate-maven/auth-api</t>
+  </si>
+  <si>
+    <t>auth-api</t>
+  </si>
+  <si>
     <t>/Users/milk/workspace/boilerplate-maven/ai-chatbot</t>
   </si>
   <si>
     <t>ai-chatbot</t>
   </si>
   <si>
-    <t>/Users/milk/workspace/boilerplate-maven/auth-api</t>
-  </si>
-  <si>
-    <t>auth-api</t>
-  </si>
-  <si>
     <t>/Users/milk/workspace/boilerplate-mvc</t>
   </si>
   <si>
     <t>unknown</t>
   </si>
   <si>
+    <t>/Users/milk/workspace/boilerplate-mvc/user</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-mvc/local/overrides</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-mvc/gradle/convention</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-mvc/common</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-mvc/api</t>
+  </si>
+  <si>
     <t>/Users/milk/workspace/boilerplate-gradle</t>
   </si>
   <si>
-    <t>/Users/milk/workspace/boilerplate-mvc/user</t>
-  </si>
-  <si>
-    <t>/Users/milk/workspace/boilerplate-mvc/common</t>
-  </si>
-  <si>
-    <t>/Users/milk/workspace/boilerplate-mvc/api</t>
-  </si>
-  <si>
     <t>/Users/milk/workspace/boilerplate-gradle/payment-service</t>
   </si>
   <si>
     <t>/Users/milk/workspace/boilerplate-gradle/order-service</t>
   </si>
   <si>
+    <t>/Users/milk/workspace/boilerplate-gradle/delivery-service</t>
+  </si>
+  <si>
     <t>/Users/milk/workspace/boilerplate-gradle/cve-service</t>
   </si>
   <si>
-    <t>/Users/milk/workspace/boilerplate-gradle/delivery-service</t>
-  </si>
-  <si>
     <t>/Users/milk/workspace/boilerplate-gradle/common-events</t>
   </si>
   <si>
-    <t>/Users/milk/workspace/boilerplate-mvc/local/overrides</t>
-  </si>
-  <si>
-    <t>/Users/milk/workspace/boilerplate-mvc/gradle/convention</t>
-  </si>
-  <si>
     <t>Project Key</t>
   </si>
   <si>
@@ -337,6 +337,9 @@
     <t>2.7.0</t>
   </si>
   <si>
+    <t>unknown:step-hts-server</t>
+  </si>
+  <si>
     <t>com.lottecard:scm-api</t>
   </si>
   <si>
@@ -370,12 +373,24 @@
     <t>2025-09-11T07:24:56.874Z</t>
   </si>
   <si>
+    <t>CVE-2025-7038</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>The LatePoint plugin for WordPress is vulnerable to Authentication Bypass due to insufficient identity verification within the steps__load_step route of the latepoint_route_call AJAX endpoint in all versions up to, and including, 5.1.94. The endpoint reads the client-supplied customer email and related customer fields before invoking the internal login handler without verifying login status, capability checks, or a valid AJAX nonce. This makes it possible for unauthenticated attackers to log into any customer’s account.</t>
+  </si>
+  <si>
+    <t>2025-09-30T04:27:07.535Z</t>
+  </si>
+  <si>
+    <t>CWE-288</t>
+  </si>
+  <si>
     <t>CVE-2025-7052</t>
   </si>
   <si>
-    <t>HIGH</t>
-  </si>
-  <si>
     <t>The LatePoint plugin for WordPress is vulnerable to Cross-Site Request Forgery in all versions up to, and including, 5.1.94. This is due to missing nonce validation on the change_password() function of its customer_cabinet__change_password AJAX route. The plugin hooks this endpoint via wp_ajax and wp_ajax_nopriv but does not verify a nonce or user capability before resetting the user’s password. This makes it possible for unauthenticated attackers who trick a logged-in customer (or, with “WP users as customers” enabled, an administrator) into visiting a malicious link to take over their account.</t>
   </si>
   <si>
@@ -385,18 +400,6 @@
     <t>CWE-352</t>
   </si>
   <si>
-    <t>CVE-2025-7038</t>
-  </si>
-  <si>
-    <t>The LatePoint plugin for WordPress is vulnerable to Authentication Bypass due to insufficient identity verification within the steps__load_step route of the latepoint_route_call AJAX endpoint in all versions up to, and including, 5.1.94. The endpoint reads the client-supplied customer email and related customer fields before invoking the internal login handler without verifying login status, capability checks, or a valid AJAX nonce. This makes it possible for unauthenticated attackers to log into any customer’s account.</t>
-  </si>
-  <si>
-    <t>2025-09-30T04:27:07.535Z</t>
-  </si>
-  <si>
-    <t>CWE-288</t>
-  </si>
-  <si>
     <t>CVE-2025-12787</t>
   </si>
   <si>
@@ -409,19 +412,10 @@
     <t>CWE-330</t>
   </si>
   <si>
-    <t>unknown:step-hts-server</t>
-  </si>
-  <si>
-    <t>com.farfarcoder:order</t>
-  </si>
-  <si>
-    <t>unknown:mcp-server</t>
-  </si>
-  <si>
-    <t>org.springframework.ai:spring-ai-starter-mcp-server-webmvc</t>
-  </si>
-  <si>
-    <t>unknown:gateway-util</t>
+    <t>unknown:partner-gateway</t>
+  </si>
+  <si>
+    <t>org.springframework.boot:spring-boot-starter-websocket</t>
   </si>
   <si>
     <t>org.springframework.boot:spring-boot-starter-webflux</t>
@@ -437,28 +431,34 @@
     <t>2025-05-19T19:25:19.350Z</t>
   </si>
   <si>
+    <t>com.farfarcoder:order</t>
+  </si>
+  <si>
+    <t>unknown:mcp-server</t>
+  </si>
+  <si>
+    <t>org.springframework.ai:spring-ai-starter-mcp-server-webmvc</t>
+  </si>
+  <si>
+    <t>unknown:gateway-util</t>
+  </si>
+  <si>
     <t>org.springframework.cloud:spring-cloud-starter-gateway-server-webflux</t>
   </si>
   <si>
     <t>unknown:gateway-domain</t>
   </si>
   <si>
-    <t>unknown:partner-gateway</t>
-  </si>
-  <si>
-    <t>org.springframework.boot:spring-boot-starter-websocket</t>
-  </si>
-  <si>
     <t>unknown:channel-gateway</t>
   </si>
   <si>
+    <t>unknown:auth-api</t>
+  </si>
+  <si>
     <t>unknown:ai-chatbot</t>
   </si>
   <si>
     <t>com.fasterxml.jackson.core:jackson-databind</t>
-  </si>
-  <si>
-    <t>unknown:auth-api</t>
   </si>
   <si>
     <t>com.farfarcoder:unknown</t>
@@ -513,20 +513,20 @@
 https://plugins.trac.wordpress.org/browser/salon-booking-system/tags/10.20/src/SLN/Plugin.php#L232</t>
   </si>
   <si>
+    <t>CVSS:3.1/AV:N/AC:L/PR:N/UI:N/S:U/C:H/I:L/A:N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.wordfence.com/threat-intel/vulnerabilities/id/d7389e17-a357-481a-8716-3a93cb6afa7c?source=cve
+https://wordpress.org/plugins/latepoint/#developers
+https://plugins.trac.wordpress.org/browser/latepoint/tags/5.1.93/latepoint.php</t>
+  </si>
+  <si>
     <t>CVSS:3.1/AV:N/AC:L/PR:N/UI:R/S:U/C:H/I:H/A:H</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.wordfence.com/threat-intel/vulnerabilities/id/df8a8ce0-7258-40ae-bf73-f8c6185fdd16?source=cve
 https://plugins.trac.wordpress.org/browser/latepoint/tags/5.1.93/lib/controllers/customer_cabinet_controller.php#L403
 https://wordpress.org/plugins/latepoint/#developers</t>
-  </si>
-  <si>
-    <t>CVSS:3.1/AV:N/AC:L/PR:N/UI:N/S:U/C:H/I:L/A:N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.wordfence.com/threat-intel/vulnerabilities/id/d7389e17-a357-481a-8716-3a93cb6afa7c?source=cve
-https://wordpress.org/plugins/latepoint/#developers
-https://plugins.trac.wordpress.org/browser/latepoint/tags/5.1.93/latepoint.php</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.wordfence.com/threat-intel/vulnerabilities/id/490dd84f-7c03-43c7-b4e1-167fa2b15c03?source=cve
@@ -1364,7 +1364,7 @@
         <v>39</v>
       </c>
       <c r="D7" s="8">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E7" s="8">
         <v>0</v>
@@ -1372,11 +1372,11 @@
       <c r="F7" s="11">
         <v>0</v>
       </c>
-      <c r="G7" s="12">
-        <v>2</v>
-      </c>
-      <c r="H7" s="13">
-        <v>7</v>
+      <c r="G7" s="11">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0</v>
       </c>
       <c r="I7" s="11">
         <v>0</v>
@@ -1393,7 +1393,7 @@
         <v>41</v>
       </c>
       <c r="D8" s="8">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E8" s="8">
         <v>0</v>
@@ -1401,11 +1401,11 @@
       <c r="F8" s="11">
         <v>0</v>
       </c>
-      <c r="G8" s="11">
-        <v>0</v>
-      </c>
-      <c r="H8" s="11">
-        <v>0</v>
+      <c r="G8" s="12">
+        <v>2</v>
+      </c>
+      <c r="H8" s="13">
+        <v>7</v>
       </c>
       <c r="I8" s="11">
         <v>0</v>
@@ -1422,7 +1422,7 @@
         <v>43</v>
       </c>
       <c r="D9" s="8">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E9" s="8">
         <v>0</v>
@@ -1433,8 +1433,8 @@
       <c r="G9" s="11">
         <v>0</v>
       </c>
-      <c r="H9" s="11">
-        <v>0</v>
+      <c r="H9" s="13">
+        <v>1</v>
       </c>
       <c r="I9" s="11">
         <v>0</v>
@@ -1451,7 +1451,7 @@
         <v>45</v>
       </c>
       <c r="D10" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E10" s="8">
         <v>0</v>
@@ -1480,7 +1480,7 @@
         <v>47</v>
       </c>
       <c r="D11" s="8">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E11" s="8">
         <v>0</v>
@@ -1491,8 +1491,8 @@
       <c r="G11" s="11">
         <v>0</v>
       </c>
-      <c r="H11" s="13">
-        <v>2</v>
+      <c r="H11" s="11">
+        <v>0</v>
       </c>
       <c r="I11" s="11">
         <v>0</v>
@@ -1509,7 +1509,7 @@
         <v>49</v>
       </c>
       <c r="D12" s="8">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E12" s="8">
         <v>0</v>
@@ -1521,7 +1521,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12" s="11">
         <v>0</v>
@@ -1538,7 +1538,7 @@
         <v>51</v>
       </c>
       <c r="D13" s="8">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E13" s="8">
         <v>0</v>
@@ -1596,7 +1596,7 @@
         <v>55</v>
       </c>
       <c r="D15" s="8">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E15" s="8">
         <v>0</v>
@@ -1625,7 +1625,7 @@
         <v>57</v>
       </c>
       <c r="D16" s="8">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E16" s="8">
         <v>0</v>
@@ -1683,7 +1683,7 @@
         <v>59</v>
       </c>
       <c r="D18" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E18" s="8">
         <v>0</v>
@@ -1712,7 +1712,7 @@
         <v>59</v>
       </c>
       <c r="D19" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E19" s="8">
         <v>0</v>
@@ -1741,7 +1741,7 @@
         <v>59</v>
       </c>
       <c r="D20" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" s="8">
         <v>0</v>
@@ -1770,7 +1770,7 @@
         <v>59</v>
       </c>
       <c r="D21" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E21" s="8">
         <v>0</v>
@@ -1799,7 +1799,7 @@
         <v>59</v>
       </c>
       <c r="D22" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E22" s="8">
         <v>0</v>
@@ -1828,7 +1828,7 @@
         <v>59</v>
       </c>
       <c r="D23" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E23" s="8">
         <v>0</v>
@@ -1857,7 +1857,7 @@
         <v>59</v>
       </c>
       <c r="D24" s="8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E24" s="8">
         <v>0</v>
@@ -1886,7 +1886,7 @@
         <v>59</v>
       </c>
       <c r="D25" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E25" s="8">
         <v>0</v>
@@ -1944,7 +1944,7 @@
         <v>59</v>
       </c>
       <c r="D27" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E27" s="8">
         <v>0</v>
@@ -2633,290 +2633,290 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C20" t="s">
-        <v>108</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E20" s="17">
-        <v>6.3</v>
+        <v>81</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="16">
+        <v>0</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="G20" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="I20" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="J20" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C21" t="s">
-        <v>108</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E21" s="17">
-        <v>6.3</v>
+        <v>87</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="16">
+        <v>0</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="G21" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="I21" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="J21" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C22" t="s">
-        <v>108</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E22" s="17">
-        <v>6.3</v>
+        <v>81</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="16">
+        <v>0</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G22" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="I22" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="J22" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C23" t="s">
-        <v>108</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E23" s="17">
-        <v>6.3</v>
+        <v>87</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="16">
+        <v>0</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G23" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="I23" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="J23" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B24" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C24" t="s">
-        <v>108</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E24" s="17">
-        <v>6.3</v>
+        <v>97</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" s="16">
+        <v>0</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="G24" t="s">
-        <v>111</v>
+        <v>59</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="I24" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="J24" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C25" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="17">
+        <v>6.3</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G25" t="s">
+        <v>112</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="I25" t="s">
+        <v>114</v>
+      </c>
+      <c r="J25" t="s">
         <v>115</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E25" s="17">
-        <v>5.3</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="G25" t="s">
-        <v>111</v>
-      </c>
-      <c r="H25" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="I25" t="s">
-        <v>117</v>
-      </c>
-      <c r="J25" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C26" t="s">
-        <v>118</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="E26" s="18">
-        <v>8.8</v>
+        <v>109</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" s="17">
+        <v>6.3</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G26" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="I26" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="J26" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C27" t="s">
-        <v>123</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="E27" s="18">
-        <v>8.2</v>
+        <v>109</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E27" s="17">
+        <v>6.3</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G27" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="I27" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="J27" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C28" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E28" s="17">
-        <v>5.3</v>
+        <v>6.3</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G28" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="I28" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="J28" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2924,31 +2924,31 @@
         <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E29" s="16">
-        <v>0</v>
+        <v>109</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E29" s="17">
+        <v>6.3</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="G29" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="H29" s="14" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="I29" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="J29" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2956,31 +2956,31 @@
         <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="C30" t="s">
-        <v>87</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E30" s="16">
-        <v>0</v>
+        <v>116</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" s="17">
+        <v>5.3</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="G30" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="I30" t="s">
-        <v>89</v>
+        <v>118</v>
       </c>
       <c r="J30" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2988,31 +2988,31 @@
         <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="C31" t="s">
-        <v>81</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E31" s="16">
-        <v>0</v>
+        <v>119</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="E31" s="18">
+        <v>8.2</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="G31" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="H31" s="14" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="I31" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="J31" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -3020,31 +3020,31 @@
         <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="C32" t="s">
-        <v>87</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E32" s="16">
-        <v>0</v>
+        <v>124</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="E32" s="18">
+        <v>8.8</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="G32" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="H32" s="14" t="s">
-        <v>88</v>
+        <v>125</v>
       </c>
       <c r="I32" t="s">
-        <v>89</v>
+        <v>126</v>
       </c>
       <c r="J32" t="s">
-        <v>86</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -3052,31 +3052,31 @@
         <v>41</v>
       </c>
       <c r="B33" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" t="s">
+        <v>128</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" s="17">
+        <v>5.3</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G33" t="s">
+        <v>112</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="I33" t="s">
+        <v>130</v>
+      </c>
+      <c r="J33" t="s">
         <v>131</v>
-      </c>
-      <c r="C33" t="s">
-        <v>97</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E33" s="16">
-        <v>0</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="G33" t="s">
-        <v>59</v>
-      </c>
-      <c r="H33" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="I33" t="s">
-        <v>100</v>
-      </c>
-      <c r="J33" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -3096,7 +3096,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>83</v>
+        <v>133</v>
       </c>
       <c r="G34" t="s">
         <v>59</v>
@@ -3128,7 +3128,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>83</v>
+        <v>133</v>
       </c>
       <c r="G35" t="s">
         <v>59</v>
@@ -3151,7 +3151,7 @@
         <v>132</v>
       </c>
       <c r="C36" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="D36" s="16" t="s">
         <v>82</v>
@@ -3160,36 +3160,36 @@
         <v>0</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>98</v>
+        <v>134</v>
       </c>
       <c r="G36" t="s">
         <v>59</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="I36" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="J36" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C37" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E37" s="16">
-        <v>0</v>
+        <v>135</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E37" s="17">
+        <v>6.1</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>134</v>
@@ -3198,10 +3198,10 @@
         <v>59</v>
       </c>
       <c r="H37" s="14" t="s">
-        <v>84</v>
+        <v>136</v>
       </c>
       <c r="I37" t="s">
-        <v>85</v>
+        <v>137</v>
       </c>
       <c r="J37" t="s">
         <v>86</v>
@@ -3209,10 +3209,10 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C38" t="s">
         <v>87</v>
@@ -3244,7 +3244,7 @@
         <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C39" t="s">
         <v>81</v>
@@ -3259,7 +3259,7 @@
         <v>83</v>
       </c>
       <c r="G39" t="s">
-        <v>103</v>
+        <v>59</v>
       </c>
       <c r="H39" s="14" t="s">
         <v>84</v>
@@ -3276,7 +3276,7 @@
         <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C40" t="s">
         <v>87</v>
@@ -3291,7 +3291,7 @@
         <v>83</v>
       </c>
       <c r="G40" t="s">
-        <v>103</v>
+        <v>59</v>
       </c>
       <c r="H40" s="14" t="s">
         <v>88</v>
@@ -3305,13 +3305,13 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C41" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="D41" s="16" t="s">
         <v>82</v>
@@ -3320,19 +3320,19 @@
         <v>0</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="G41" t="s">
         <v>59</v>
       </c>
       <c r="H41" s="14" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="I41" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="J41" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -3340,28 +3340,28 @@
         <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C42" t="s">
-        <v>137</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E42" s="17">
-        <v>6.1</v>
+        <v>81</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E42" s="16">
+        <v>0</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="G42" t="s">
         <v>59</v>
       </c>
       <c r="H42" s="14" t="s">
-        <v>138</v>
+        <v>84</v>
       </c>
       <c r="I42" t="s">
-        <v>139</v>
+        <v>85</v>
       </c>
       <c r="J42" t="s">
         <v>86</v>
@@ -3372,7 +3372,7 @@
         <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C43" t="s">
         <v>87</v>
@@ -3384,7 +3384,7 @@
         <v>0</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="G43" t="s">
         <v>59</v>
@@ -3404,7 +3404,7 @@
         <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C44" t="s">
         <v>81</v>
@@ -3416,10 +3416,10 @@
         <v>0</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>140</v>
+        <v>83</v>
       </c>
       <c r="G44" t="s">
-        <v>59</v>
+        <v>103</v>
       </c>
       <c r="H44" s="14" t="s">
         <v>84</v>
@@ -3436,28 +3436,28 @@
         <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C45" t="s">
-        <v>137</v>
-      </c>
-      <c r="D45" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E45" s="17">
-        <v>6.1</v>
+        <v>87</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E45" s="16">
+        <v>0</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>140</v>
+        <v>83</v>
       </c>
       <c r="G45" t="s">
-        <v>59</v>
+        <v>103</v>
       </c>
       <c r="H45" s="14" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="I45" t="s">
-        <v>139</v>
+        <v>89</v>
       </c>
       <c r="J45" t="s">
         <v>86</v>
@@ -3465,13 +3465,13 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C46" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D46" s="16" t="s">
         <v>82</v>
@@ -3480,16 +3480,16 @@
         <v>0</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="G46" t="s">
         <v>59</v>
       </c>
       <c r="H46" s="14" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I46" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J46" t="s">
         <v>86</v>
@@ -3503,25 +3503,25 @@
         <v>141</v>
       </c>
       <c r="C47" t="s">
-        <v>81</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E47" s="16">
-        <v>0</v>
+        <v>135</v>
+      </c>
+      <c r="D47" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E47" s="17">
+        <v>6.1</v>
       </c>
       <c r="F47" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="G47" t="s">
+        <v>59</v>
+      </c>
+      <c r="H47" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="G47" t="s">
-        <v>59</v>
-      </c>
-      <c r="H47" s="14" t="s">
-        <v>84</v>
-      </c>
       <c r="I47" t="s">
-        <v>85</v>
+        <v>137</v>
       </c>
       <c r="J47" t="s">
         <v>86</v>
@@ -3535,25 +3535,25 @@
         <v>141</v>
       </c>
       <c r="C48" t="s">
-        <v>137</v>
-      </c>
-      <c r="D48" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E48" s="17">
-        <v>6.1</v>
+        <v>87</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E48" s="16">
+        <v>0</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G48" t="s">
         <v>59</v>
       </c>
       <c r="H48" s="14" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="I48" t="s">
-        <v>139</v>
+        <v>89</v>
       </c>
       <c r="J48" t="s">
         <v>86</v>
@@ -3567,7 +3567,7 @@
         <v>141</v>
       </c>
       <c r="C49" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D49" s="16" t="s">
         <v>82</v>
@@ -3576,16 +3576,16 @@
         <v>0</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="G49" t="s">
         <v>59</v>
       </c>
       <c r="H49" s="14" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I49" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J49" t="s">
         <v>86</v>
@@ -3593,31 +3593,31 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
+        <v>141</v>
+      </c>
+      <c r="C50" t="s">
+        <v>135</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E50" s="17">
+        <v>6.1</v>
+      </c>
+      <c r="F50" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="C50" t="s">
-        <v>81</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E50" s="16">
-        <v>0</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>143</v>
-      </c>
       <c r="G50" t="s">
         <v>59</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>84</v>
+        <v>136</v>
       </c>
       <c r="I50" t="s">
-        <v>85</v>
+        <v>137</v>
       </c>
       <c r="J50" t="s">
         <v>86</v>
@@ -3625,10 +3625,10 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C51" t="s">
         <v>87</v>
@@ -3640,7 +3640,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G51" t="s">
         <v>59</v>
@@ -3660,7 +3660,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C52" t="s">
         <v>81</v>
@@ -3672,7 +3672,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G52" t="s">
         <v>59</v>
@@ -3692,28 +3692,28 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C53" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E53" s="17">
         <v>6.1</v>
       </c>
       <c r="F53" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="G53" t="s">
+        <v>59</v>
+      </c>
+      <c r="H53" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="G53" t="s">
-        <v>59</v>
-      </c>
-      <c r="H53" s="14" t="s">
-        <v>138</v>
-      </c>
       <c r="I53" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J53" t="s">
         <v>86</v>
@@ -3724,7 +3724,7 @@
         <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C54" t="s">
         <v>87</v>
@@ -3736,7 +3736,7 @@
         <v>0</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G54" t="s">
         <v>59</v>
@@ -3768,7 +3768,7 @@
         <v>0</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G55" t="s">
         <v>59</v>
@@ -3791,25 +3791,25 @@
         <v>144</v>
       </c>
       <c r="C56" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E56" s="17">
         <v>6.1</v>
       </c>
       <c r="F56" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="G56" t="s">
+        <v>59</v>
+      </c>
+      <c r="H56" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="G56" t="s">
-        <v>59</v>
-      </c>
-      <c r="H56" s="14" t="s">
-        <v>138</v>
-      </c>
       <c r="I56" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J56" t="s">
         <v>86</v>
@@ -3832,7 +3832,7 @@
         <v>0</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G57" t="s">
         <v>59</v>
@@ -3864,7 +3864,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G58" t="s">
         <v>59</v>
@@ -3887,25 +3887,25 @@
         <v>144</v>
       </c>
       <c r="C59" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E59" s="17">
         <v>6.1</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G59" t="s">
         <v>59</v>
       </c>
       <c r="H59" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I59" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J59" t="s">
         <v>86</v>
@@ -3928,7 +3928,7 @@
         <v>0</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G60" t="s">
         <v>59</v>
@@ -3960,10 +3960,10 @@
         <v>0</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="G61" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H61" s="14" t="s">
         <v>84</v>
@@ -3992,10 +3992,10 @@
         <v>0</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="G62" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H62" s="14" t="s">
         <v>88</v>
@@ -4015,7 +4015,7 @@
         <v>145</v>
       </c>
       <c r="C63" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D63" s="16" t="s">
         <v>82</v>
@@ -4024,27 +4024,27 @@
         <v>0</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>146</v>
+        <v>98</v>
       </c>
       <c r="G63" t="s">
         <v>59</v>
       </c>
       <c r="H63" s="14" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="I63" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="J63" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B64" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C64" t="s">
         <v>81</v>
@@ -4056,10 +4056,10 @@
         <v>0</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="G64" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H64" s="14" t="s">
         <v>84</v>
@@ -4073,10 +4073,10 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B65" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C65" t="s">
         <v>87</v>
@@ -4088,10 +4088,10 @@
         <v>0</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="G65" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H65" s="14" t="s">
         <v>88</v>
@@ -4108,31 +4108,31 @@
         <v>57</v>
       </c>
       <c r="B66" t="s">
+        <v>146</v>
+      </c>
+      <c r="C66" t="s">
+        <v>90</v>
+      </c>
+      <c r="D66" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E66" s="16">
+        <v>0</v>
+      </c>
+      <c r="F66" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="C66" t="s">
-        <v>81</v>
-      </c>
-      <c r="D66" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E66" s="16">
-        <v>0</v>
-      </c>
-      <c r="F66" s="8" t="s">
-        <v>105</v>
-      </c>
       <c r="G66" t="s">
-        <v>106</v>
+        <v>59</v>
       </c>
       <c r="H66" s="14" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="I66" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="J66" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -4140,10 +4140,10 @@
         <v>57</v>
       </c>
       <c r="B67" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C67" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D67" s="16" t="s">
         <v>82</v>
@@ -4158,10 +4158,10 @@
         <v>106</v>
       </c>
       <c r="H67" s="14" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I67" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J67" t="s">
         <v>86</v>
@@ -4172,10 +4172,10 @@
         <v>57</v>
       </c>
       <c r="B68" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C68" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D68" s="16" t="s">
         <v>82</v>
@@ -4184,19 +4184,19 @@
         <v>0</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="G68" t="s">
-        <v>59</v>
+        <v>106</v>
       </c>
       <c r="H68" s="14" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="I68" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="J68" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
@@ -4492,10 +4492,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C6" s="8">
         <v>6.3</v>
@@ -4504,13 +4504,13 @@
         <v>160</v>
       </c>
       <c r="E6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="G6" t="s">
         <v>114</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="G6" t="s">
-        <v>113</v>
       </c>
       <c r="I6" s="14" t="s">
         <v>161</v>
@@ -4518,10 +4518,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C7" s="8">
         <v>5.3</v>
@@ -4530,13 +4530,13 @@
         <v>162</v>
       </c>
       <c r="E7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I7" s="14" t="s">
         <v>163</v>
@@ -4544,25 +4544,25 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C8" s="8">
-        <v>8.8</v>
+        <v>8.2</v>
       </c>
       <c r="D8" t="s">
         <v>164</v>
       </c>
       <c r="E8" t="s">
+        <v>123</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" t="s">
         <v>122</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="G8" t="s">
-        <v>121</v>
       </c>
       <c r="I8" s="14" t="s">
         <v>165</v>
@@ -4570,25 +4570,25 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C9" s="8">
-        <v>8.2</v>
+        <v>8.8</v>
       </c>
       <c r="D9" t="s">
         <v>166</v>
       </c>
       <c r="E9" t="s">
+        <v>127</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G9" t="s">
         <v>126</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="G9" t="s">
-        <v>125</v>
       </c>
       <c r="I9" s="14" t="s">
         <v>167</v>
@@ -4596,10 +4596,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C10" s="8">
         <v>5.3</v>
@@ -4608,13 +4608,13 @@
         <v>162</v>
       </c>
       <c r="E10" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="G10" t="s">
         <v>130</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="G10" t="s">
-        <v>129</v>
       </c>
       <c r="I10" s="14" t="s">
         <v>168</v>
@@ -4622,10 +4622,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C11" s="8">
         <v>6.1</v>
@@ -4637,10 +4637,10 @@
         <v>86</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I11" s="14" t="s">
         <v>170</v>

</xml_diff>

<commit_message>
add and modify : cve gradle maven ant
</commit_message>
<xml_diff>
--- a/vulnerability-scanner/output/vulnerability-dashboard.xlsx
+++ b/vulnerability-scanner/output/vulnerability-dashboard.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="182">
   <si>
     <t>🛡️ Vulnerability Scan Summary</t>
   </si>
@@ -22,7 +22,7 @@
     <t>Scan Date:</t>
   </si>
   <si>
-    <t>2025. 12. 9. 오전 11:09:00</t>
+    <t>2025. 12. 9. 오후 1:29:08</t>
   </si>
   <si>
     <t>Scanner Version:</t>
@@ -227,6 +227,12 @@
   </si>
   <si>
     <t>/Users/milk/workspace/boilerplate-gradle/common-events</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/-bmjs/vulnerability-scanner/test-ant-project</t>
+  </si>
+  <si>
+    <t>test-ant</t>
   </si>
   <si>
     <t>Project Key</t>
@@ -468,6 +474,27 @@
   </si>
   <si>
     <t>unknown:unknown</t>
+  </si>
+  <si>
+    <t>unknown:test-ant</t>
+  </si>
+  <si>
+    <t>CVE-2022-21704</t>
+  </si>
+  <si>
+    <t>unknown:log4j</t>
+  </si>
+  <si>
+    <t>1.2.17</t>
+  </si>
+  <si>
+    <t>log4js-node is a port of log4js to node.js. In affected versions default file permissions for log files created by the file, fileSync and dateFile appenders are world-readable (in unix). This could cause problems if log files contain sensitive information. This would affect any users that have not supplied their own permissions for the files via the mode parameter in the config. Users are advised to update.</t>
+  </si>
+  <si>
+    <t>2022-01-19T00:00:00.000Z</t>
+  </si>
+  <si>
+    <t>CWE-276</t>
   </si>
   <si>
     <t>CVSS Vector</t>
@@ -538,6 +565,14 @@
   <si>
     <t xml:space="preserve">https://github.com/symfony/ux/security/advisories/GHSA-5j3w-5pcr-f8hg
 https://github.com/symfony/ux/commit/b5d1c85995c128cb926d47a96cfbfbd500b643a8</t>
+  </si>
+  <si>
+    <t>CVSS:3.1/AV:L/AC:L/PR:L/UI:N/S:U/C:H/I:N/A:N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/log4js-node/log4js-node/security/advisories/GHSA-82v2-mx6x-wq7q
+https://github.com/log4js-node/log4js-node/pull/1141/commits/8042252861a1b65adb66931fdf702ead34fa9b76
+https://github.com/log4js-node/streamroller/pull/87</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1087,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1076,7 +1111,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -1089,7 +1124,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="3">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1097,7 +1132,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1105,7 +1140,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1137,7 +1172,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="6">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1162,7 +1197,7 @@
   <sheetPr>
     <tabColor rgb="FF4FACFE"/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1991,8 +2026,37 @@
         <v>0</v>
       </c>
     </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="8">
+        <v>1</v>
+      </c>
+      <c r="E29" s="8">
+        <v>0</v>
+      </c>
+      <c r="F29" s="11">
+        <v>0</v>
+      </c>
+      <c r="G29" s="11">
+        <v>0</v>
+      </c>
+      <c r="H29" s="13">
+        <v>1</v>
+      </c>
+      <c r="I29" s="11">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I28"/>
+  <autoFilter ref="A1:I29"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
@@ -2003,7 +2067,7 @@
   <sheetPr>
     <tabColor rgb="FFFF8C00"/>
   </sheetPr>
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2028,31 +2092,31 @@
         <v>20</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2060,31 +2124,31 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E2" s="16">
         <v>0</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G2" t="s">
         <v>59</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2092,31 +2156,31 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E3" s="16">
         <v>0</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G3" t="s">
         <v>59</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2124,31 +2188,31 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E4" s="16">
         <v>0</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G4" t="s">
         <v>59</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="J4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2156,31 +2220,31 @@
         <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E5" s="16">
         <v>0</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G5" t="s">
         <v>59</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2188,31 +2252,31 @@
         <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E6" s="16">
         <v>0</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G6" t="s">
         <v>59</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2220,31 +2284,31 @@
         <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E7" s="16">
         <v>0</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G7" t="s">
         <v>59</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2252,31 +2316,31 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E8" s="16">
         <v>0</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G8" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -2284,31 +2348,31 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E9" s="16">
         <v>0</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G9" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I9" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2316,31 +2380,31 @@
         <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E10" s="16">
         <v>0</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I10" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J10" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2348,31 +2412,31 @@
         <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E11" s="16">
         <v>0</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G11" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I11" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J11" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2380,31 +2444,31 @@
         <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E12" s="16">
         <v>0</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G12" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -2412,31 +2476,31 @@
         <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C13" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E13" s="16">
         <v>0</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G13" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I13" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J13" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2444,31 +2508,31 @@
         <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C14" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E14" s="16">
         <v>0</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G14" t="s">
         <v>59</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I14" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2476,31 +2540,31 @@
         <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C15" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E15" s="16">
         <v>0</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G15" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I15" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J15" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2508,31 +2572,31 @@
         <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E16" s="16">
         <v>0</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G16" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I16" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J16" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -2540,31 +2604,31 @@
         <v>39</v>
       </c>
       <c r="B17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="16">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" s="16">
-        <v>0</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>105</v>
-      </c>
       <c r="G17" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J17" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -2572,31 +2636,31 @@
         <v>39</v>
       </c>
       <c r="B18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="16">
+        <v>0</v>
+      </c>
+      <c r="F18" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C18" t="s">
-        <v>87</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" s="16">
-        <v>0</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>105</v>
-      </c>
       <c r="G18" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I18" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J18" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -2604,31 +2668,31 @@
         <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E19" s="16">
         <v>0</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G19" t="s">
         <v>59</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I19" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J19" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -2636,31 +2700,31 @@
         <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C20" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E20" s="16">
         <v>0</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G20" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I20" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J20" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2668,31 +2732,31 @@
         <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E21" s="16">
         <v>0</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G21" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I21" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J21" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -2700,31 +2764,31 @@
         <v>41</v>
       </c>
       <c r="B22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="16">
+        <v>0</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" t="s">
         <v>108</v>
       </c>
-      <c r="C22" t="s">
-        <v>81</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" s="16">
-        <v>0</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="G22" t="s">
-        <v>106</v>
-      </c>
       <c r="H22" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I22" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J22" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2732,31 +2796,31 @@
         <v>41</v>
       </c>
       <c r="B23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="16">
+        <v>0</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G23" t="s">
         <v>108</v>
       </c>
-      <c r="C23" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" s="16">
-        <v>0</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="G23" t="s">
-        <v>106</v>
-      </c>
       <c r="H23" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I23" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J23" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -2764,31 +2828,31 @@
         <v>41</v>
       </c>
       <c r="B24" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C24" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E24" s="16">
         <v>0</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G24" t="s">
         <v>59</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I24" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J24" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -2796,31 +2860,31 @@
         <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C25" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E25" s="17">
         <v>6.3</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G25" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I25" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="J25" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -2828,31 +2892,31 @@
         <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C26" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E26" s="17">
         <v>6.3</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G26" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I26" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="J26" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2860,31 +2924,31 @@
         <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E27" s="17">
         <v>6.3</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G27" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="J27" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2892,31 +2956,31 @@
         <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C28" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E28" s="17">
         <v>6.3</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G28" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I28" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="J28" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2924,31 +2988,31 @@
         <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C29" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E29" s="17">
         <v>6.3</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G29" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H29" s="14" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I29" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="J29" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2956,31 +3020,31 @@
         <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C30" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E30" s="17">
         <v>5.3</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G30" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H30" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="I30" t="s">
+        <v>120</v>
+      </c>
+      <c r="J30" t="s">
         <v>117</v>
-      </c>
-      <c r="I30" t="s">
-        <v>118</v>
-      </c>
-      <c r="J30" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2988,31 +3052,31 @@
         <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C31" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E31" s="18">
         <v>8.2</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G31" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H31" s="14" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I31" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="J31" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -3020,31 +3084,31 @@
         <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C32" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E32" s="18">
         <v>8.8</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G32" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H32" s="14" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="I32" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="J32" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -3052,31 +3116,31 @@
         <v>41</v>
       </c>
       <c r="B33" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C33" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E33" s="17">
         <v>5.3</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G33" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H33" s="14" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I33" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="J33" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -3084,31 +3148,31 @@
         <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C34" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E34" s="16">
         <v>0</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G34" t="s">
         <v>59</v>
       </c>
       <c r="H34" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I34" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J34" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3116,31 +3180,31 @@
         <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C35" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E35" s="16">
         <v>0</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G35" t="s">
         <v>59</v>
       </c>
       <c r="H35" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I35" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J35" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -3148,31 +3212,31 @@
         <v>43</v>
       </c>
       <c r="B36" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C36" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E36" s="16">
         <v>0</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G36" t="s">
         <v>59</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I36" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J36" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -3180,31 +3244,31 @@
         <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C37" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E37" s="17">
         <v>6.1</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G37" t="s">
         <v>59</v>
       </c>
       <c r="H37" s="14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="I37" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="J37" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -3212,31 +3276,31 @@
         <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C38" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E38" s="16">
         <v>0</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G38" t="s">
         <v>59</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I38" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J38" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -3244,31 +3308,31 @@
         <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C39" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E39" s="16">
         <v>0</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G39" t="s">
         <v>59</v>
       </c>
       <c r="H39" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I39" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J39" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -3276,31 +3340,31 @@
         <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C40" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E40" s="16">
         <v>0</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G40" t="s">
         <v>59</v>
       </c>
       <c r="H40" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I40" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J40" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -3308,31 +3372,31 @@
         <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C41" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E41" s="16">
         <v>0</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G41" t="s">
         <v>59</v>
       </c>
       <c r="H41" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I41" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J41" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -3340,31 +3404,31 @@
         <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C42" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E42" s="16">
         <v>0</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G42" t="s">
         <v>59</v>
       </c>
       <c r="H42" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I42" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J42" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -3372,31 +3436,31 @@
         <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C43" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E43" s="16">
         <v>0</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G43" t="s">
         <v>59</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I43" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J43" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -3404,31 +3468,31 @@
         <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C44" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E44" s="16">
         <v>0</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G44" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I44" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J44" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -3436,31 +3500,31 @@
         <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C45" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E45" s="16">
         <v>0</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G45" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H45" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I45" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J45" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -3468,31 +3532,31 @@
         <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C46" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E46" s="16">
         <v>0</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G46" t="s">
         <v>59</v>
       </c>
       <c r="H46" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I46" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J46" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -3500,31 +3564,31 @@
         <v>49</v>
       </c>
       <c r="B47" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C47" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E47" s="17">
         <v>6.1</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G47" t="s">
         <v>59</v>
       </c>
       <c r="H47" s="14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="I47" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="J47" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -3532,31 +3596,31 @@
         <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C48" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E48" s="16">
         <v>0</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G48" t="s">
         <v>59</v>
       </c>
       <c r="H48" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I48" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J48" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -3564,31 +3628,31 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C49" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E49" s="16">
         <v>0</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G49" t="s">
         <v>59</v>
       </c>
       <c r="H49" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I49" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J49" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -3596,31 +3660,31 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C50" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E50" s="17">
         <v>6.1</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G50" t="s">
         <v>59</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="I50" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="J50" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -3628,31 +3692,31 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C51" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E51" s="16">
         <v>0</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G51" t="s">
         <v>59</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I51" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J51" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -3660,31 +3724,31 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C52" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E52" s="16">
         <v>0</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G52" t="s">
         <v>59</v>
       </c>
       <c r="H52" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I52" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J52" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -3692,31 +3756,31 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C53" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E53" s="17">
         <v>6.1</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G53" t="s">
         <v>59</v>
       </c>
       <c r="H53" s="14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="I53" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="J53" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -3724,31 +3788,31 @@
         <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C54" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E54" s="16">
         <v>0</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G54" t="s">
         <v>59</v>
       </c>
       <c r="H54" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I54" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J54" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -3756,31 +3820,31 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C55" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E55" s="16">
         <v>0</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G55" t="s">
         <v>59</v>
       </c>
       <c r="H55" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I55" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J55" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -3788,31 +3852,31 @@
         <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C56" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E56" s="17">
         <v>6.1</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G56" t="s">
         <v>59</v>
       </c>
       <c r="H56" s="14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="I56" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="J56" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
@@ -3820,31 +3884,31 @@
         <v>53</v>
       </c>
       <c r="B57" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C57" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D57" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E57" s="16">
         <v>0</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G57" t="s">
         <v>59</v>
       </c>
       <c r="H57" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I57" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J57" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -3852,31 +3916,31 @@
         <v>53</v>
       </c>
       <c r="B58" t="s">
+        <v>146</v>
+      </c>
+      <c r="C58" t="s">
+        <v>83</v>
+      </c>
+      <c r="D58" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E58" s="16">
+        <v>0</v>
+      </c>
+      <c r="F58" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C58" t="s">
-        <v>81</v>
-      </c>
-      <c r="D58" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E58" s="16">
-        <v>0</v>
-      </c>
-      <c r="F58" s="8" t="s">
-        <v>142</v>
-      </c>
       <c r="G58" t="s">
         <v>59</v>
       </c>
       <c r="H58" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I58" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J58" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
@@ -3884,31 +3948,31 @@
         <v>53</v>
       </c>
       <c r="B59" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C59" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E59" s="17">
         <v>6.1</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G59" t="s">
         <v>59</v>
       </c>
       <c r="H59" s="14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="I59" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="J59" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -3916,31 +3980,31 @@
         <v>53</v>
       </c>
       <c r="B60" t="s">
+        <v>146</v>
+      </c>
+      <c r="C60" t="s">
+        <v>89</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E60" s="16">
+        <v>0</v>
+      </c>
+      <c r="F60" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C60" t="s">
-        <v>87</v>
-      </c>
-      <c r="D60" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E60" s="16">
-        <v>0</v>
-      </c>
-      <c r="F60" s="8" t="s">
-        <v>142</v>
-      </c>
       <c r="G60" t="s">
         <v>59</v>
       </c>
       <c r="H60" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I60" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J60" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
@@ -3948,31 +4012,31 @@
         <v>55</v>
       </c>
       <c r="B61" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C61" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E61" s="16">
         <v>0</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G61" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H61" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I61" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J61" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
@@ -3980,31 +4044,31 @@
         <v>55</v>
       </c>
       <c r="B62" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C62" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E62" s="16">
         <v>0</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G62" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H62" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I62" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J62" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
@@ -4012,31 +4076,31 @@
         <v>55</v>
       </c>
       <c r="B63" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C63" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E63" s="16">
         <v>0</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G63" t="s">
         <v>59</v>
       </c>
       <c r="H63" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I63" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J63" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -4044,31 +4108,31 @@
         <v>57</v>
       </c>
       <c r="B64" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C64" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D64" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E64" s="16">
         <v>0</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G64" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H64" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I64" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J64" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
@@ -4076,31 +4140,31 @@
         <v>57</v>
       </c>
       <c r="B65" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C65" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E65" s="16">
         <v>0</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G65" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H65" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I65" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J65" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
@@ -4108,31 +4172,31 @@
         <v>57</v>
       </c>
       <c r="B66" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C66" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E66" s="16">
         <v>0</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G66" t="s">
         <v>59</v>
       </c>
       <c r="H66" s="14" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I66" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="J66" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -4140,31 +4204,31 @@
         <v>57</v>
       </c>
       <c r="B67" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C67" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E67" s="16">
         <v>0</v>
       </c>
       <c r="F67" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G67" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H67" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I67" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J67" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
@@ -4172,31 +4236,31 @@
         <v>57</v>
       </c>
       <c r="B68" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C68" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E68" s="16">
         <v>0</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G68" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H68" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I68" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J68" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
@@ -4204,31 +4268,31 @@
         <v>59</v>
       </c>
       <c r="B69" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C69" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D69" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E69" s="16">
         <v>0</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G69" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H69" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I69" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J69" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
@@ -4236,31 +4300,31 @@
         <v>59</v>
       </c>
       <c r="B70" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C70" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D70" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E70" s="16">
         <v>0</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G70" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H70" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I70" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J70" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
@@ -4268,31 +4332,31 @@
         <v>59</v>
       </c>
       <c r="B71" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C71" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D71" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E71" s="16">
         <v>0</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G71" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H71" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I71" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J71" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
@@ -4300,35 +4364,67 @@
         <v>59</v>
       </c>
       <c r="B72" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C72" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D72" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E72" s="16">
         <v>0</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G72" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H72" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I72" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J72" t="s">
-        <v>86</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>153</v>
+      </c>
+      <c r="C73" t="s">
+        <v>154</v>
+      </c>
+      <c r="D73" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="E73" s="17">
+        <v>5.5</v>
+      </c>
+      <c r="F73" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="G73" t="s">
+        <v>156</v>
+      </c>
+      <c r="H73" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="I73" t="s">
+        <v>158</v>
+      </c>
+      <c r="J73" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J72"/>
+  <autoFilter ref="A1:J73"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
@@ -4339,7 +4435,7 @@
   <sheetPr>
     <tabColor rgb="FFFFD700"/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4359,295 +4455,321 @@
   <sheetData>
     <row r="1" ht="25" customHeight="1" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="E1" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="15" t="s">
-        <v>77</v>
-      </c>
       <c r="G1" s="9" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C2" s="8">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="E2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>84</v>
-      </c>
       <c r="G2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C3" s="8">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="E3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C4" s="8">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="E4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="F4" s="14" t="s">
-        <v>92</v>
-      </c>
       <c r="G4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C5" s="8">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="E5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="F5" s="14" t="s">
-        <v>99</v>
-      </c>
       <c r="G5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C6" s="8">
         <v>6.3</v>
       </c>
       <c r="D6" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="E6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>113</v>
-      </c>
       <c r="G6" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C7" s="8">
         <v>5.3</v>
       </c>
       <c r="D7" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="E7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G7" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C8" s="8">
         <v>8.2</v>
       </c>
       <c r="D8" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="E8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>121</v>
-      </c>
       <c r="G8" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C9" s="8">
         <v>8.8</v>
       </c>
       <c r="D9" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="E9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F9" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="F9" s="14" t="s">
-        <v>125</v>
-      </c>
       <c r="G9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C10" s="8">
         <v>5.3</v>
       </c>
       <c r="D10" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="E10" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="F10" s="14" t="s">
-        <v>129</v>
-      </c>
       <c r="G10" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C11" s="8">
         <v>6.1</v>
       </c>
       <c r="D11" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="E11" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G11" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>170</v>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="8">
+        <v>5.5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>180</v>
+      </c>
+      <c r="E12" t="s">
+        <v>159</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="G12" t="s">
+        <v>158</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I11"/>
+  <autoFilter ref="A1:I12"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
modify : 오류 해결
</commit_message>
<xml_diff>
--- a/vulnerability-scanner/output/vulnerability-dashboard.xlsx
+++ b/vulnerability-scanner/output/vulnerability-dashboard.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
   <si>
     <t>🛡️ Vulnerability Scan Summary</t>
   </si>
@@ -22,7 +22,7 @@
     <t>Scan Date:</t>
   </si>
   <si>
-    <t>2025. 12. 10. 오후 3:04:02</t>
+    <t>2025. 12. 10. 오후 4:06:02</t>
   </si>
   <si>
     <t>Scanner Version:</t>
@@ -100,7 +100,10 @@
     <t>🔵 Low</t>
   </si>
   <si>
-    <t>c-project</t>
+    <t>java-project</t>
+  </si>
+  <si>
+    <t>my-app</t>
   </si>
   <si>
     <t>Project Key</t>
@@ -130,6 +133,27 @@
     <t>CWEs</t>
   </si>
   <si>
+    <t>com.example:my-app</t>
+  </si>
+  <si>
+    <t>CVE-2024-JAVA-TEST</t>
+  </si>
+  <si>
+    <t>CRITICAL</t>
+  </si>
+  <si>
+    <t>org.springframework:spring-core</t>
+  </si>
+  <si>
+    <t>5.3.10</t>
+  </si>
+  <si>
+    <t>Vulnerability in mocked spring-core</t>
+  </si>
+  <si>
+    <t>2024-01-01T00:00:00.000Z</t>
+  </si>
+  <si>
     <t>CVSS Vector</t>
   </si>
   <si>
@@ -140,13 +164,16 @@
   </si>
   <si>
     <t>References</t>
+  </si>
+  <si>
+    <t>CVSS:3.1/AV:N/AC:L/PR:N/UI:N/S:U/C:H/I:H/A:H</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -187,6 +214,10 @@
       <color rgb="FFFFFFFF"/>
     </font>
     <font>
+      <b/>
+      <color rgb="FF3B3B"/>
+    </font>
+    <font>
       <color rgb="FF808080"/>
     </font>
   </fonts>
@@ -215,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -238,11 +269,17 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -627,7 +664,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -635,7 +672,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -651,7 +688,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -664,7 +701,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -672,7 +709,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -680,7 +717,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -696,7 +733,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -737,7 +774,7 @@
   <sheetPr>
     <tabColor rgb="FF4FACFE"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -788,61 +825,32 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" s="8">
         <v>0</v>
       </c>
       <c r="F2" s="11">
+        <v>1</v>
+      </c>
+      <c r="G2" s="12">
         <v>0</v>
       </c>
-      <c r="G2" s="11">
+      <c r="H2" s="12">
         <v>0</v>
       </c>
-      <c r="H2" s="11">
+      <c r="I2" s="12">
         <v>0</v>
       </c>
-      <c r="I2" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="8">
-        <v>2</v>
-      </c>
-      <c r="E3" s="8">
-        <v>0</v>
-      </c>
-      <c r="F3" s="11">
-        <v>0</v>
-      </c>
-      <c r="G3" s="11">
-        <v>0</v>
-      </c>
-      <c r="H3" s="11">
-        <v>0</v>
-      </c>
-      <c r="I3" s="11">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I3"/>
+  <autoFilter ref="A1:I2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
@@ -853,7 +861,7 @@
   <sheetPr>
     <tabColor rgb="FFFF8C00"/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -868,7 +876,7 @@
     <col min="4" max="5" width="12" style="8" customWidth="1"/>
     <col min="6" max="6" width="40" style="8" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="80" style="12" customWidth="1"/>
+    <col min="8" max="8" width="80" style="13" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
   </cols>
@@ -878,35 +886,67 @@
         <v>20</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>37</v>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="15">
+        <v>9.8</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1"/>
+  <autoFilter ref="A1:J2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
@@ -917,7 +957,7 @@
   <sheetPr>
     <tabColor rgb="FFFFD700"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -930,42 +970,71 @@
     <col min="2" max="3" width="12" style="8" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="80" style="12" customWidth="1"/>
+    <col min="6" max="6" width="80" style="13" customWidth="1"/>
     <col min="7" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="60" style="12" customWidth="1"/>
+    <col min="9" max="9" width="60" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>35</v>
+      <c r="F1" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H1" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="B2" s="8" t="s">
         <v>41</v>
       </c>
+      <c r="C2" s="8">
+        <v>9.8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1"/>
+  <autoFilter ref="A1:I2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
modify : 코드 수정
</commit_message>
<xml_diff>
--- a/vulnerability-scanner/output/vulnerability-dashboard.xlsx
+++ b/vulnerability-scanner/output/vulnerability-dashboard.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
   <si>
     <t>🛡️ Vulnerability Scan Summary</t>
   </si>
@@ -22,7 +22,7 @@
     <t>Scan Date:</t>
   </si>
   <si>
-    <t>2025. 12. 12. 오후 1:04:55</t>
+    <t>2025. 12. 12. 오후 1:57:44</t>
   </si>
   <si>
     <t>Scanner Version:</t>
@@ -100,7 +100,7 @@
     <t>🔵 Low</t>
   </si>
   <si>
-    <t>repro-tika</t>
+    <t>/Users/milk/workspace/-bmjs/vulnerability-scanner/repro-tika</t>
   </si>
   <si>
     <t>my-app</t>
@@ -154,6 +154,27 @@
     <t>2025-12-04T16:17:24.980Z</t>
   </si>
   <si>
+    <t>CVE-2025-54988</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>org.apache.tika:tika-parser-pdf-module</t>
+  </si>
+  <si>
+    <t>3.2.1</t>
+  </si>
+  <si>
+    <t>Critical XXE in Apache Tika (tika-parser-pdf-module).</t>
+  </si>
+  <si>
+    <t>2025-08-20T20:08:49.481Z</t>
+  </si>
+  <si>
+    <t>CWE-611</t>
+  </si>
+  <si>
     <t>CVSS Vector</t>
   </si>
   <si>
@@ -167,13 +188,16 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>CVSS:3.1/AV:L/AC:L/PR:N/UI:N/S:U/C:H/I:H/A:H</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -218,6 +242,10 @@
     </font>
     <font>
       <b/>
+      <color rgb="FF8C00"/>
+    </font>
+    <font>
+      <b/>
       <color rgb="FFA0A0A0"/>
     </font>
   </fonts>
@@ -246,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -269,13 +297,19 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -685,7 +719,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -698,7 +732,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -714,7 +748,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -738,7 +772,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -828,7 +862,7 @@
         <v>29</v>
       </c>
       <c r="D2" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="8">
         <v>0</v>
@@ -836,8 +870,8 @@
       <c r="F2" s="11">
         <v>0</v>
       </c>
-      <c r="G2" s="11">
-        <v>0</v>
+      <c r="G2" s="12">
+        <v>1</v>
       </c>
       <c r="H2" s="11">
         <v>0</v>
@@ -858,7 +892,7 @@
   <sheetPr>
     <tabColor rgb="FFFF8C00"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -873,7 +907,7 @@
     <col min="4" max="5" width="12" style="8" customWidth="1"/>
     <col min="6" max="6" width="40" style="8" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="80" style="12" customWidth="1"/>
+    <col min="8" max="8" width="80" style="13" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
   </cols>
@@ -900,7 +934,7 @@
       <c r="G1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="14" t="s">
         <v>36</v>
       </c>
       <c r="I1" s="9" t="s">
@@ -920,10 +954,10 @@
       <c r="C2" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="15">
         <v>0</v>
       </c>
       <c r="F2" s="8" t="s">
@@ -932,7 +966,7 @@
       <c r="G2" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="13" t="s">
         <v>44</v>
       </c>
       <c r="I2" t="s">
@@ -942,8 +976,40 @@
         <v>14</v>
       </c>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="16">
+        <v>8.4</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J2"/>
+  <autoFilter ref="A1:J3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
@@ -954,7 +1020,7 @@
   <sheetPr>
     <tabColor rgb="FFFFD700"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -967,9 +1033,9 @@
     <col min="2" max="3" width="12" style="8" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="80" style="12" customWidth="1"/>
+    <col min="6" max="6" width="80" style="13" customWidth="1"/>
     <col min="7" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="60" style="12" customWidth="1"/>
+    <col min="9" max="9" width="60" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -983,22 +1049,22 @@
         <v>33</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="14" t="s">
         <v>36</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>49</v>
+        <v>55</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1012,12 +1078,12 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="13" t="s">
         <v>44</v>
       </c>
       <c r="G2" t="s">
@@ -1026,12 +1092,41 @@
       <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="13" t="s">
         <v>14</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="8">
+        <v>8.4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I2"/>
+  <autoFilter ref="A1:I3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
modify : code 수정
</commit_message>
<xml_diff>
--- a/vulnerability-scanner/output/vulnerability-dashboard.xlsx
+++ b/vulnerability-scanner/output/vulnerability-dashboard.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
   <si>
     <t>🛡️ Vulnerability Scan Summary</t>
   </si>
@@ -22,7 +22,7 @@
     <t>Scan Date:</t>
   </si>
   <si>
-    <t>2025. 12. 12. 오후 1:57:44</t>
+    <t>2025. 12. 12. 오후 2:38:17</t>
   </si>
   <si>
     <t>Scanner Version:</t>
@@ -139,21 +139,27 @@
     <t>CVE-2025-66516</t>
   </si>
   <si>
-    <t>NONE</t>
+    <t>CRITICAL</t>
   </si>
   <si>
     <t>org.apache.tika:tika-core</t>
   </si>
   <si>
-    <t>1.14</t>
-  </si>
-  <si>
-    <t>No description available</t>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Critical XXE in Apache Tika tika-core (1.13-3.2.1), tika-pdf-module (2.0.0-3.2.1) and tika-parsers (1.13-1.28.5) modules on all platforms allows an attacker to carry out XML External Entity injection via a crafted XFA file inside of a PDF. 
+This CVE covers the same vulnerability as in CVE-2025-54988. However, this CVE expands the scope of affected packages in two ways. 
+First, while the entrypoint for the vulnerability was the tika-parser-pdf-module as reported in CVE-2025-54988, the vulnerability and its fix were in tika-core. Users who upgraded the tika-parser-pdf-module but did not upgrade tika-core to &gt;= 3.2.2 would still be vulnerable. 
+Second, the original report failed to mention that in the 1.x Tika releases, the PDFParser was in the "org.apache.tika:tika-parsers" module.</t>
   </si>
   <si>
     <t>2025-12-04T16:17:24.980Z</t>
   </si>
   <si>
+    <t>CWE-611</t>
+  </si>
+  <si>
     <t>CVE-2025-54988</t>
   </si>
   <si>
@@ -172,9 +178,6 @@
     <t>2025-08-20T20:08:49.481Z</t>
   </si>
   <si>
-    <t>CWE-611</t>
-  </si>
-  <si>
     <t>CVSS Vector</t>
   </si>
   <si>
@@ -187,7 +190,11 @@
     <t>References</t>
   </si>
   <si>
-    <t>N/A</t>
+    <t>CVSS:4.0/AV:N/AC:L/AT:N/PR:N/UI:N/VC:H/VI:H/VA:H/SC:H/SI:H/SA:H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://lists.apache.org/thread/s5x3k93nhbkqzztp1olxotoyjpdlps9k
+https://cve.org/CVERecord?id=CVE-2025-54988</t>
   </si>
   <si>
     <t>CVSS:3.1/AV:L/AC:L/PR:N/UI:N/S:U/C:H/I:H/A:H</t>
@@ -238,15 +245,15 @@
       <color rgb="FFFFFFFF"/>
     </font>
     <font>
-      <color rgb="FF808080"/>
+      <b/>
+      <color rgb="FF3B3B"/>
     </font>
     <font>
       <b/>
       <color rgb="FF8C00"/>
     </font>
     <font>
-      <b/>
-      <color rgb="FFA0A0A0"/>
+      <color rgb="FF808080"/>
     </font>
   </fonts>
   <fills count="3">
@@ -274,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -300,13 +307,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -732,7 +742,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -764,7 +774,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -868,15 +878,15 @@
         <v>0</v>
       </c>
       <c r="F2" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G2" s="12">
         <v>1</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="13">
         <v>0</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="13">
         <v>0</v>
       </c>
     </row>
@@ -892,7 +902,7 @@
   <sheetPr>
     <tabColor rgb="FFFF8C00"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -907,7 +917,7 @@
     <col min="4" max="5" width="12" style="8" customWidth="1"/>
     <col min="6" max="6" width="40" style="8" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="80" style="13" customWidth="1"/>
+    <col min="8" max="8" width="80" style="14" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
   </cols>
@@ -934,7 +944,7 @@
       <c r="G1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="15" t="s">
         <v>36</v>
       </c>
       <c r="I1" s="9" t="s">
@@ -954,11 +964,11 @@
       <c r="C2" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="15">
-        <v>0</v>
+      <c r="E2" s="16">
+        <v>10</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>42</v>
@@ -966,14 +976,14 @@
       <c r="G2" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="14" t="s">
         <v>44</v>
       </c>
       <c r="I2" t="s">
         <v>45</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -984,32 +994,64 @@
         <v>39</v>
       </c>
       <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="17">
+        <v>8.4</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="16">
-        <v>8.4</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" t="s">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="16">
+        <v>10</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="G4" t="s">
         <v>50</v>
       </c>
-      <c r="I3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" t="s">
-        <v>52</v>
+      <c r="H4" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J3"/>
+  <autoFilter ref="A1:J4"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
@@ -1033,9 +1075,9 @@
     <col min="2" max="3" width="12" style="8" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="80" style="13" customWidth="1"/>
+    <col min="6" max="6" width="80" style="14" customWidth="1"/>
     <col min="7" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="60" style="13" customWidth="1"/>
+    <col min="9" max="9" width="60" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1054,7 +1096,7 @@
       <c r="E1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="15" t="s">
         <v>36</v>
       </c>
       <c r="G1" s="9" t="s">
@@ -1063,7 +1105,7 @@
       <c r="H1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="15" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1075,15 +1117,15 @@
         <v>41</v>
       </c>
       <c r="C2" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>44</v>
       </c>
       <c r="G2" t="s">
@@ -1092,36 +1134,36 @@
       <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="13" t="s">
-        <v>14</v>
+      <c r="I2" s="14" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C3" s="8">
         <v>8.4</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" t="s">
         <v>52</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" t="s">
-        <v>51</v>
       </c>
       <c r="H3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="14" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modify : uiux 수정
</commit_message>
<xml_diff>
--- a/vulnerability-scanner/output/vulnerability-dashboard.xlsx
+++ b/vulnerability-scanner/output/vulnerability-dashboard.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="147">
   <si>
     <t>🛡️ Vulnerability Scan Summary</t>
   </si>
@@ -22,7 +22,7 @@
     <t>Scan Date:</t>
   </si>
   <si>
-    <t>2025. 12. 15. 오후 1:45:45</t>
+    <t>2025. 12. 16. 오후 2:22:48</t>
   </si>
   <si>
     <t>Scanner Version:</t>
@@ -100,12 +100,156 @@
     <t>🔵 Low</t>
   </si>
   <si>
+    <t>/Users/milk/workspace/cicd</t>
+  </si>
+  <si>
+    <t>cicd</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven-21</t>
+  </si>
+  <si>
+    <t>mobileid</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven</t>
+  </si>
+  <si>
+    <t>boilerplate-maven</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/web-common</t>
+  </si>
+  <si>
+    <t>web-common</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/tour-api</t>
+  </si>
+  <si>
+    <t>tour-api</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/step-hts-server</t>
+  </si>
+  <si>
+    <t>step-hts-server</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/scm-api</t>
+  </si>
+  <si>
+    <t>scm-api</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/partner-gateway</t>
+  </si>
+  <si>
+    <t>partner-gateway</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/order</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/mcp-server</t>
+  </si>
+  <si>
+    <t>mcp-server</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/gateway-util</t>
+  </si>
+  <si>
+    <t>gateway-util</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/gateway-domain</t>
+  </si>
+  <si>
+    <t>gateway-domain</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/channel-gateway</t>
+  </si>
+  <si>
+    <t>channel-gateway</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/auth-api</t>
+  </si>
+  <si>
+    <t>auth-api</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/ai-chatbot</t>
+  </si>
+  <si>
+    <t>ai-chatbot</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/-bmjs/vulnerability-scanner/test-project</t>
+  </si>
+  <si>
+    <t>test-app</t>
+  </si>
+  <si>
     <t>/Users/milk/workspace/-bmjs/vulnerability-scanner/repro-tika</t>
   </si>
   <si>
     <t>my-app</t>
   </si>
   <si>
+    <t>/Users/milk/workspace/-bmjs/vulnerability-scanner/java-project</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-mvc</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-mvc/user</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-mvc/local/overrides</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-mvc/gradle/convention</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-mvc/common</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-mvc/api</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-gradle</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-gradle/payment-service</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-gradle/order-service</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-gradle/delivery-service</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-gradle/cve-service</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-gradle/common-events</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/-bmjs/vulnerability-scanner/c-project</t>
+  </si>
+  <si>
+    <t>c-project</t>
+  </si>
+  <si>
     <t>Project Key</t>
   </si>
   <si>
@@ -133,49 +277,172 @@
     <t>CWEs</t>
   </si>
   <si>
+    <t>unknown:partner-gateway</t>
+  </si>
+  <si>
+    <t>CVE-2025-48924</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>org.apache.commons:commons-lang3</t>
+  </si>
+  <si>
+    <t>3.13.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncontrolled Recursion vulnerability in Apache Commons Lang.
+This issue affects Apache Commons Lang: Starting with commons-lang:commons-lang 2.0 to 2.6, and, from org.apache.commons:commons-lang3 3.0 before 3.18.0.
+The methods ClassUtils.getClass(...) can throw StackOverflowError on very long inputs. Because an Error is usually not handled by applications and libraries, a 
+StackOverflowError could cause an application to stop.
+Users are recommended to upgrade to version 3.18.0, which fixes the issue.</t>
+  </si>
+  <si>
+    <t>2025-07-11T14:56:58.049Z</t>
+  </si>
+  <si>
+    <t>CWE-674</t>
+  </si>
+  <si>
+    <t>unknown:channel-gateway</t>
+  </si>
+  <si>
     <t>com.example:my-app</t>
   </si>
   <si>
-    <t>CVE-2025-66516</t>
-  </si>
-  <si>
-    <t>CRITICAL</t>
-  </si>
-  <si>
-    <t>org.apache.tika:tika-core</t>
-  </si>
-  <si>
-    <t>1.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Critical XXE in Apache Tika tika-core (1.13-3.2.1), tika-pdf-module (2.0.0-3.2.1) and tika-parsers (1.13-1.28.5) modules on all platforms allows an attacker to carry out XML External Entity injection via a crafted XFA file inside of a PDF. 
-This CVE covers the same vulnerability as in CVE-2025-54988. However, this CVE expands the scope of affected packages in two ways. 
-First, while the entrypoint for the vulnerability was the tika-parser-pdf-module as reported in CVE-2025-54988, the vulnerability and its fix were in tika-core. Users who upgraded the tika-parser-pdf-module but did not upgrade tika-core to &gt;= 3.2.2 would still be vulnerable. 
-Second, the original report failed to mention that in the 1.x Tika releases, the PDFParser was in the "org.apache.tika:tika-parsers" module.</t>
-  </si>
-  <si>
-    <t>2025-12-04T16:17:24.980Z</t>
+    <t>CVE-2025-54988</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>org.apache.tika:tika-parser-pdf-module</t>
+  </si>
+  <si>
+    <t>3.2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Critical XXE in Apache Tika (tika-parser-pdf-module) in Apache Tika 1.13 through and including 3.2.1 on all platforms allows an attacker to carry out XML External Entity injection via a crafted XFA file inside of a PDF. An attacker may be able to read sensitive data or trigger malicious requests to internal resources or third-party servers. Note that the tika-parser-pdf-module is used as a dependency in several Tika packages including at least: tika-parsers-standard-modules, tika-parsers-standard-package, tika-app, tika-grpc and tika-server-standard.
+Users are recommended to upgrade to version 3.2.2, which fixes this issue.</t>
+  </si>
+  <si>
+    <t>2025-08-20T20:08:49.481Z</t>
   </si>
   <si>
     <t>CWE-611</t>
   </si>
   <si>
-    <t>CVE-2025-54988</t>
-  </si>
-  <si>
-    <t>HIGH</t>
-  </si>
-  <si>
-    <t>org.apache.tika:tika-parser-pdf-module</t>
-  </si>
-  <si>
-    <t>3.2.1</t>
-  </si>
-  <si>
-    <t>Critical XXE in Apache Tika (tika-parser-pdf-module).</t>
-  </si>
-  <si>
-    <t>2025-08-20T20:08:49.481Z</t>
+    <t>CVE-2018-1258</t>
+  </si>
+  <si>
+    <t>org.springframework:spring-core</t>
+  </si>
+  <si>
+    <t>5.3.10</t>
+  </si>
+  <si>
+    <t>Spring Framework version 5.0.5 when used in combination with any versions of Spring Security contains an authorization bypass when using method security. An unauthorized malicious user can gain unauthorized access to methods that should be restricted.</t>
+  </si>
+  <si>
+    <t>2018-05-11T20:00:00Z</t>
+  </si>
+  <si>
+    <t>CVE-2018-15756</t>
+  </si>
+  <si>
+    <t>Spring Framework, version 5.1, versions 5.0.x prior to 5.0.10, versions 4.3.x prior to 4.3.20, and older unsupported versions on the 4.2.x branch provide support for range requests when serving static resources through the ResourceHttpRequestHandler, or starting in 5.0 when an annotated controller returns an org.springframework.core.io.Resource. A malicious user (or attacker) can add a range header with a high number of ranges, or with wide ranges that overlap, or both, for a denial of service attack. This vulnerability affects applications that depend on either spring-webmvc or spring-webflux. Such applications must also have a registration for serving static resources (e.g. JS, CSS, images, and others), or have an annotated controller that returns an org.springframework.core.io.Resource. Spring Boot applications that depend on spring-boot-starter-web or spring-boot-starter-webflux are ready to serve static resources out of the box and are therefore vulnerable.</t>
+  </si>
+  <si>
+    <t>2018-10-18T22:00:00Z</t>
+  </si>
+  <si>
+    <t>CVE-2025-41242</t>
+  </si>
+  <si>
+    <t>MEDIUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spring Framework MVC applications can be vulnerable to a “Path Traversal Vulnerability” when deployed on a non-compliant Servlet container.
+An application can be vulnerable when all the following are true:
+  *  the application is deployed as a WAR or with an embedded Servlet container
+  *  the Servlet container  does not reject suspicious sequences https://jakarta.ee/specifications/servlet/6.1/jakarta-servlet-spec-6.1.html#uri-path-canonicalization 
+  *  the application  serves static resources https://docs.spring.io/spring-framework/reference/web/webmvc/mvc-config/static-resources.html#page-title  with Spring resource handling
+We have verified that applications deployed on Apache Tomcat or Eclipse Jetty are not vulnerable, as long as default security features are not disabled in the configuration. Because we cannot check exploits against all Servlet containers and configuration variants, we strongly recommend upgrading your application.</t>
+  </si>
+  <si>
+    <t>2025-08-18T08:47:07.427Z</t>
+  </si>
+  <si>
+    <t>CVE-2025-41249</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Spring Framework annotation detection mechanism may not correctly resolve annotations on methods within type hierarchies with a parameterized super type with unbounded generics. This can be an issue if such annotations are used for authorization decisions.
+Your application may be affected by this if you are using Spring Security's @EnableMethodSecurity feature.
+You are not affected by this if you are not using @EnableMethodSecurity or if you do not use security annotations on methods in generic superclasses or generic interfaces.
+This CVE is published in conjunction with  CVE-2025-41248 https://spring.io/security/cve-2025-41248 .</t>
+  </si>
+  <si>
+    <t>2025-09-16T10:15:34.118Z</t>
+  </si>
+  <si>
+    <t>CVE-2025-41254</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STOMP over WebSocket applications may be vulnerable to a security bypass that allows an attacker to send unauthorized messages.
+Affected Spring Products and VersionsSpring Framework:
+  *  6.2.0 - 6.2.11
+  *  6.1.0 - 6.1.23
+  *  6.0.x - 6.0.29
+  *  5.3.0 - 5.3.45
+  *  Older, unsupported versions are also affected.
+MitigationUsers of affected versions should upgrade to the corresponding fixed version.
+Affected version(s)Fix versionAvailability6.2.x6.2.12OSS6.1.x6.1.24 Commercial https://enterprise.spring.io/ 6.0.xN/A Out of support https://spring.io/projects/spring-framework#support 5.3.x5.3.46 Commercial https://enterprise.spring.io/ No further mitigation steps are necessary.
+CreditThis vulnerability was discovered and responsibly reported by Jannis Kaiser.</t>
+  </si>
+  <si>
+    <t>2025-10-16T14:48:37.350Z</t>
+  </si>
+  <si>
+    <t>CWE-352</t>
+  </si>
+  <si>
+    <t>CVE-2025-22233</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CVE-2024-38820 ensured Locale-independent, lowercase conversion for both the configured disallowedFields patterns and for request parameter names. However, there are still cases where it is possible to bypass the disallowedFields checks.
+Affected Spring Products and Versions
+Spring Framework:
+  *  6.2.0 - 6.2.6
+  *  6.1.0 - 6.1.19
+  *  6.0.0 - 6.0.27
+  *  5.3.0 - 5.3.42
+  *  Older, unsupported versions are also affected
+Mitigation
+Users of affected versions should upgrade to the corresponding fixed version.
+Affected version(s)Fix Version Availability 6.2.x
+ 6.2.7
+OSS6.1.x
+ 6.1.20
+OSS6.0.x
+ 6.0.28
+ Commercial https://enterprise.spring.io/ 5.3.x
+ 5.3.43
+ Commercial https://enterprise.spring.io/ 
+No further mitigation steps are necessary.
+Generally, we recommend using a dedicated model object with properties only for data binding, or using constructor binding since constructor arguments explicitly declare what to bind together with turning off setter binding through the declarativeBinding flag. See the Model Design section in the reference documentation.
+For setting binding, prefer the use of allowedFields (an explicit list) over disallowedFields.
+Credit
+This issue was responsibly reported by the TERASOLUNA Framework Development Team from NTT DATA Group Corporation.</t>
+  </si>
+  <si>
+    <t>2025-05-16T19:14:07.500Z</t>
+  </si>
+  <si>
+    <t>CWE-20</t>
   </si>
   <si>
     <t>CVSS Vector</t>
@@ -190,21 +457,61 @@
     <t>References</t>
   </si>
   <si>
-    <t>CVSS:4.0/AV:N/AC:L/AT:N/PR:N/UI:N/VC:H/VI:H/VA:H/SC:H/SI:H/SA:H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://lists.apache.org/thread/s5x3k93nhbkqzztp1olxotoyjpdlps9k
-https://cve.org/CVERecord?id=CVE-2025-54988</t>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>https://lists.apache.org/thread/bgv0lpswokgol11tloxnjfzdl7yrc1g1</t>
   </si>
   <si>
     <t>CVSS:3.1/AV:L/AC:L/PR:N/UI:N/S:U/C:H/I:H/A:H</t>
+  </si>
+  <si>
+    <t>https://lists.apache.org/thread/8xn3rqy6kz5b3l1t83kcofkw0w4mmj1w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.securityfocus.com/bid/104222
+http://www.securitytracker.com/id/1041888
+http://www.securitytracker.com/id/1041896</t>
+  </si>
+  <si>
+    <t>CVSS:3.0/AV:N/AC:L/PR:N/UI:N/S:U/C:N/I:N/A:H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.securityfocus.com/bid/105703
+https://lists.apache.org/thread.html/a3071e11c6fbd593022074ec1b4693f6d948c2b02cfa4a5d854aed68%40%3Cissues.activemq.apache.org%3E
+https://lists.apache.org/thread.html/339fd112517e4873695b5115b96acdddbfc8f83b10598528d37c7d12%40%3Cissues.activemq.apache.org%3E</t>
+  </si>
+  <si>
+    <t>CVSS:3.1/AV:N/AC:H/PR:N/UI:N/S:U/C:H/I:N/A:N</t>
+  </si>
+  <si>
+    <t>http://spring.io/security/cve-2025-41242</t>
+  </si>
+  <si>
+    <t>CVSS:3.1/AV:N/AC:L/PR:N/UI:N/S:U/C:H/I:N/A:N</t>
+  </si>
+  <si>
+    <t>https://spring.io/security/cve-2025-41249</t>
+  </si>
+  <si>
+    <t>CVSS:3.1/AV:N/AC:L/PR:N/UI:R/S:U/C:N/I:L/A:N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://spring.io/security/cve/2025-41254
+https://nvd.nist.gov/vuln-metrics/cvss/v3-calculator?vector=AV:N/AC:L/PR:N/UI:R/S:U/C:N/I:L/A:N&amp;version=3.1</t>
+  </si>
+  <si>
+    <t>CVSS:3.1/AV:N/AC:H/PR:L/UI:N/S:U/C:N/I:L/A:N</t>
+  </si>
+  <si>
+    <t>https://nvd.nist.gov/vuln-metrics/cvss/v3-calculator?vector=AV:N/AC:H/PR:L/UI:N/S:U/C:N/I:L/A:N&amp;version=3.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -245,15 +552,23 @@
       <color rgb="FFFFFFFF"/>
     </font>
     <font>
-      <b/>
-      <color rgb="FF3B3B"/>
+      <color rgb="FF808080"/>
     </font>
     <font>
       <b/>
       <color rgb="FF8C00"/>
     </font>
     <font>
-      <color rgb="FF808080"/>
+      <b/>
+      <color rgb="FFD700"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="4A9EFF"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FFA0A0A0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -281,7 +596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -310,16 +625,25 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -705,7 +1029,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -713,7 +1037,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -721,7 +1045,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -729,7 +1053,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3">
-        <v>2</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -742,7 +1066,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="3">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -750,7 +1074,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -758,7 +1082,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="3">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -774,7 +1098,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -782,7 +1106,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -790,7 +1114,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -798,7 +1122,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +1139,7 @@
   <sheetPr>
     <tabColor rgb="FF4FACFE"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -872,26 +1196,896 @@
         <v>29</v>
       </c>
       <c r="D2" s="8">
+        <v>6</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0</v>
+      </c>
+      <c r="F2" s="11">
+        <v>0</v>
+      </c>
+      <c r="G2" s="11">
+        <v>0</v>
+      </c>
+      <c r="H2" s="11">
+        <v>0</v>
+      </c>
+      <c r="I2" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="8">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0</v>
+      </c>
+      <c r="G3" s="11">
+        <v>0</v>
+      </c>
+      <c r="H3" s="11">
+        <v>0</v>
+      </c>
+      <c r="I3" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11">
+        <v>0</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="8">
+        <v>3</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="11">
+        <v>0</v>
+      </c>
+      <c r="G5" s="11">
+        <v>0</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0</v>
+      </c>
+      <c r="I5" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="8">
+        <v>11</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0</v>
+      </c>
+      <c r="G6" s="11">
+        <v>0</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0</v>
+      </c>
+      <c r="I6" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="8">
+        <v>11</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0</v>
+      </c>
+      <c r="G7" s="11">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0</v>
+      </c>
+      <c r="I7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="8">
+        <v>24</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0</v>
+      </c>
+      <c r="G8" s="11">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0</v>
+      </c>
+      <c r="I8" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="8">
+        <v>18</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0</v>
+      </c>
+      <c r="I9" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="8">
+        <v>6</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0</v>
+      </c>
+      <c r="G10" s="11">
+        <v>0</v>
+      </c>
+      <c r="H10" s="11">
+        <v>0</v>
+      </c>
+      <c r="I10" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="8">
+        <v>5</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0</v>
+      </c>
+      <c r="F11" s="11">
+        <v>0</v>
+      </c>
+      <c r="G11" s="11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="8">
+        <v>11</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0</v>
+      </c>
+      <c r="F12" s="11">
+        <v>0</v>
+      </c>
+      <c r="G12" s="11">
+        <v>0</v>
+      </c>
+      <c r="H12" s="11">
+        <v>0</v>
+      </c>
+      <c r="I12" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="8">
+        <v>3</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0</v>
+      </c>
+      <c r="F13" s="11">
+        <v>0</v>
+      </c>
+      <c r="G13" s="11">
+        <v>0</v>
+      </c>
+      <c r="H13" s="11">
+        <v>0</v>
+      </c>
+      <c r="I13" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="8">
+        <v>17</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0</v>
+      </c>
+      <c r="F14" s="11">
+        <v>0</v>
+      </c>
+      <c r="G14" s="11">
+        <v>0</v>
+      </c>
+      <c r="H14" s="11">
+        <v>0</v>
+      </c>
+      <c r="I14" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="8">
+        <v>18</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0</v>
+      </c>
+      <c r="F15" s="11">
+        <v>0</v>
+      </c>
+      <c r="G15" s="11">
+        <v>0</v>
+      </c>
+      <c r="H15" s="11">
+        <v>0</v>
+      </c>
+      <c r="I15" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="8">
+        <v>11</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0</v>
+      </c>
+      <c r="F16" s="11">
+        <v>0</v>
+      </c>
+      <c r="G16" s="11">
+        <v>0</v>
+      </c>
+      <c r="H16" s="11">
+        <v>0</v>
+      </c>
+      <c r="I16" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="8">
+        <v>1</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0</v>
+      </c>
+      <c r="F17" s="11">
+        <v>0</v>
+      </c>
+      <c r="G17" s="11">
+        <v>0</v>
+      </c>
+      <c r="H17" s="11">
+        <v>0</v>
+      </c>
+      <c r="I17" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="8">
         <v>2</v>
       </c>
-      <c r="E2" s="8">
-        <v>0</v>
-      </c>
-      <c r="F2" s="11">
+      <c r="E18" s="8">
+        <v>0</v>
+      </c>
+      <c r="F18" s="11">
+        <v>0</v>
+      </c>
+      <c r="G18" s="12">
+        <v>1</v>
+      </c>
+      <c r="H18" s="11">
+        <v>0</v>
+      </c>
+      <c r="I18" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="8">
+        <v>1</v>
+      </c>
+      <c r="E19" s="8">
+        <v>0</v>
+      </c>
+      <c r="F19" s="11">
+        <v>0</v>
+      </c>
+      <c r="G19" s="12">
         <v>2</v>
       </c>
-      <c r="G2" s="12">
+      <c r="H19" s="13">
+        <v>2</v>
+      </c>
+      <c r="I19" s="14">
         <v>1</v>
       </c>
-      <c r="H2" s="13">
-        <v>0</v>
-      </c>
-      <c r="I2" s="13">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="8">
+        <v>0</v>
+      </c>
+      <c r="E20" s="8">
+        <v>0</v>
+      </c>
+      <c r="F20" s="11">
+        <v>0</v>
+      </c>
+      <c r="G20" s="11">
+        <v>0</v>
+      </c>
+      <c r="H20" s="11">
+        <v>0</v>
+      </c>
+      <c r="I20" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="8">
+        <v>2</v>
+      </c>
+      <c r="E21" s="8">
+        <v>0</v>
+      </c>
+      <c r="F21" s="11">
+        <v>0</v>
+      </c>
+      <c r="G21" s="11">
+        <v>0</v>
+      </c>
+      <c r="H21" s="11">
+        <v>0</v>
+      </c>
+      <c r="I21" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0</v>
+      </c>
+      <c r="E22" s="8">
+        <v>0</v>
+      </c>
+      <c r="F22" s="11">
+        <v>0</v>
+      </c>
+      <c r="G22" s="11">
+        <v>0</v>
+      </c>
+      <c r="H22" s="11">
+        <v>0</v>
+      </c>
+      <c r="I22" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0</v>
+      </c>
+      <c r="E23" s="8">
+        <v>0</v>
+      </c>
+      <c r="F23" s="11">
+        <v>0</v>
+      </c>
+      <c r="G23" s="11">
+        <v>0</v>
+      </c>
+      <c r="H23" s="11">
+        <v>0</v>
+      </c>
+      <c r="I23" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="8">
+        <v>1</v>
+      </c>
+      <c r="E24" s="8">
+        <v>0</v>
+      </c>
+      <c r="F24" s="11">
+        <v>0</v>
+      </c>
+      <c r="G24" s="11">
+        <v>0</v>
+      </c>
+      <c r="H24" s="11">
+        <v>0</v>
+      </c>
+      <c r="I24" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="8">
+        <v>3</v>
+      </c>
+      <c r="E25" s="8">
+        <v>0</v>
+      </c>
+      <c r="F25" s="11">
+        <v>0</v>
+      </c>
+      <c r="G25" s="11">
+        <v>0</v>
+      </c>
+      <c r="H25" s="11">
+        <v>0</v>
+      </c>
+      <c r="I25" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="8">
+        <v>0</v>
+      </c>
+      <c r="E26" s="8">
+        <v>0</v>
+      </c>
+      <c r="F26" s="11">
+        <v>0</v>
+      </c>
+      <c r="G26" s="11">
+        <v>0</v>
+      </c>
+      <c r="H26" s="11">
+        <v>0</v>
+      </c>
+      <c r="I26" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="8">
+        <v>0</v>
+      </c>
+      <c r="E27" s="8">
+        <v>0</v>
+      </c>
+      <c r="F27" s="11">
+        <v>0</v>
+      </c>
+      <c r="G27" s="11">
+        <v>0</v>
+      </c>
+      <c r="H27" s="11">
+        <v>0</v>
+      </c>
+      <c r="I27" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="8">
+        <v>2</v>
+      </c>
+      <c r="E28" s="8">
+        <v>0</v>
+      </c>
+      <c r="F28" s="11">
+        <v>0</v>
+      </c>
+      <c r="G28" s="11">
+        <v>0</v>
+      </c>
+      <c r="H28" s="11">
+        <v>0</v>
+      </c>
+      <c r="I28" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="8">
+        <v>0</v>
+      </c>
+      <c r="E29" s="8">
+        <v>0</v>
+      </c>
+      <c r="F29" s="11">
+        <v>0</v>
+      </c>
+      <c r="G29" s="11">
+        <v>0</v>
+      </c>
+      <c r="H29" s="11">
+        <v>0</v>
+      </c>
+      <c r="I29" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="8">
+        <v>3</v>
+      </c>
+      <c r="E30" s="8">
+        <v>0</v>
+      </c>
+      <c r="F30" s="11">
+        <v>0</v>
+      </c>
+      <c r="G30" s="11">
+        <v>0</v>
+      </c>
+      <c r="H30" s="11">
+        <v>0</v>
+      </c>
+      <c r="I30" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="8">
+        <v>0</v>
+      </c>
+      <c r="E31" s="8">
+        <v>0</v>
+      </c>
+      <c r="F31" s="11">
+        <v>0</v>
+      </c>
+      <c r="G31" s="11">
+        <v>0</v>
+      </c>
+      <c r="H31" s="11">
+        <v>0</v>
+      </c>
+      <c r="I31" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="8">
+        <v>1</v>
+      </c>
+      <c r="E32" s="8">
+        <v>0</v>
+      </c>
+      <c r="F32" s="11">
+        <v>0</v>
+      </c>
+      <c r="G32" s="11">
+        <v>0</v>
+      </c>
+      <c r="H32" s="11">
+        <v>0</v>
+      </c>
+      <c r="I32" s="11">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I2"/>
+  <autoFilter ref="A1:I32"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
@@ -902,7 +2096,7 @@
   <sheetPr>
     <tabColor rgb="FFFF8C00"/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -918,7 +2112,7 @@
     <col min="5" max="6" width="12" style="8" customWidth="1"/>
     <col min="7" max="7" width="40" style="8" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="80" style="14" customWidth="1"/>
+    <col min="9" max="9" width="80" style="15" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
   </cols>
@@ -931,140 +2125,350 @@
         <v>20</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>36</v>
+        <v>83</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>84</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="16">
-        <v>10</v>
+        <v>88</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" s="17">
+        <v>0</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="H2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>44</v>
+        <v>91</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="J2" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="K2" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="F3" s="17">
-        <v>8.4</v>
+        <v>0</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="H3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>51</v>
+        <v>91</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="J3" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="K3" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="16">
-        <v>10</v>
+        <v>97</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="18">
+        <v>8.4</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="H4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>44</v>
+        <v>100</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="J4" t="s">
-        <v>45</v>
+        <v>102</v>
       </c>
       <c r="K4" t="s">
-        <v>46</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="17">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" t="s">
+        <v>106</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="J5" t="s">
+        <v>108</v>
+      </c>
+      <c r="K5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="18">
+        <v>7.5</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" t="s">
+        <v>106</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="J6" t="s">
+        <v>111</v>
+      </c>
+      <c r="K6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" s="19">
+        <v>5.9</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="J7" t="s">
+        <v>115</v>
+      </c>
+      <c r="K7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="18">
+        <v>7.5</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H8" t="s">
+        <v>106</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="J8" t="s">
+        <v>118</v>
+      </c>
+      <c r="K8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" s="19">
+        <v>4.3</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H9" t="s">
+        <v>106</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="J9" t="s">
+        <v>121</v>
+      </c>
+      <c r="K9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="F10" s="20">
+        <v>3.1</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10" t="s">
+        <v>106</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="J10" t="s">
+        <v>126</v>
+      </c>
+      <c r="K10" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K4"/>
+  <autoFilter ref="A1:K10"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
@@ -1075,7 +2479,7 @@
   <sheetPr>
     <tabColor rgb="FFFFD700"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1088,100 +2492,274 @@
     <col min="2" max="3" width="12" style="8" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="80" style="14" customWidth="1"/>
+    <col min="6" max="6" width="80" style="15" customWidth="1"/>
     <col min="7" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="60" style="14" customWidth="1"/>
+    <col min="9" max="9" width="60" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>36</v>
+        <v>86</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>84</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>56</v>
+        <v>130</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
       <c r="C2" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>132</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>44</v>
+        <v>94</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="14" t="s">
-        <v>58</v>
+      <c r="I2" s="15" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>97</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="C3" s="8">
         <v>8.4</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>134</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>51</v>
+        <v>103</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="H3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" t="s">
         <v>14</v>
       </c>
+      <c r="F4" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="8">
+        <v>5.9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="G6" t="s">
+        <v>115</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="8">
+        <v>4.3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" t="s">
+        <v>121</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="8">
+        <v>3.1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" t="s">
+        <v>127</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="G9" t="s">
+        <v>126</v>
+      </c>
+      <c r="H9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>146</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I3"/>
+  <autoFilter ref="A1:I9"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
add : cves 취악점 수정
</commit_message>
<xml_diff>
--- a/vulnerability-scanner/output/vulnerability-dashboard.xlsx
+++ b/vulnerability-scanner/output/vulnerability-dashboard.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="152">
   <si>
     <t>🛡️ Vulnerability Scan Summary</t>
   </si>
@@ -22,7 +22,7 @@
     <t>Scan Date:</t>
   </si>
   <si>
-    <t>2025. 12. 18. 오후 5:43:27</t>
+    <t>2025. 12. 19. 오후 5:21:46</t>
   </si>
   <si>
     <t>Scanner Version:</t>
@@ -215,6 +215,12 @@
   </si>
   <si>
     <t>/Users/milk/workspace/-bmjs/vulnerability-scanner/java-project</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/-bmjs/vulnerability-scanner/cve-service</t>
+  </si>
+  <si>
+    <t>cve-service</t>
   </si>
   <si>
     <t>/Users/milk/workspace/boilerplate-mvc</t>
@@ -1038,7 +1044,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1046,7 +1052,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1062,7 +1068,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -1148,7 +1154,7 @@
   <sheetPr>
     <tabColor rgb="FF4FACFE"/>
   </sheetPr>
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1779,16 +1785,16 @@
         <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E20" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F20" s="8">
         <v>0</v>
@@ -1808,7 +1814,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
         <v>39</v>
@@ -1820,7 +1826,7 @@
         <v>39</v>
       </c>
       <c r="E21" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F21" s="8">
         <v>0</v>
@@ -1840,7 +1846,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B22" t="s">
         <v>39</v>
@@ -1852,7 +1858,7 @@
         <v>39</v>
       </c>
       <c r="E22" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F22" s="8">
         <v>0</v>
@@ -1872,7 +1878,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
         <v>39</v>
@@ -1904,7 +1910,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
         <v>39</v>
@@ -1916,7 +1922,7 @@
         <v>39</v>
       </c>
       <c r="E24" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" s="8">
         <v>0</v>
@@ -1936,7 +1942,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B25" t="s">
         <v>39</v>
@@ -1948,7 +1954,7 @@
         <v>39</v>
       </c>
       <c r="E25" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F25" s="8">
         <v>0</v>
@@ -1968,7 +1974,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B26" t="s">
         <v>39</v>
@@ -1977,10 +1983,10 @@
         <v>39</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E26" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F26" s="8">
         <v>0</v>
@@ -2000,7 +2006,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B27" t="s">
         <v>39</v>
@@ -2032,7 +2038,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s">
         <v>39</v>
@@ -2044,7 +2050,7 @@
         <v>31</v>
       </c>
       <c r="E28" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F28" s="8">
         <v>0</v>
@@ -2064,7 +2070,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B29" t="s">
         <v>39</v>
@@ -2076,7 +2082,7 @@
         <v>31</v>
       </c>
       <c r="E29" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F29" s="8">
         <v>0</v>
@@ -2096,7 +2102,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B30" t="s">
         <v>39</v>
@@ -2105,10 +2111,10 @@
         <v>39</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E30" s="8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F30" s="8">
         <v>0</v>
@@ -2128,7 +2134,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B31" t="s">
         <v>39</v>
@@ -2140,7 +2146,7 @@
         <v>39</v>
       </c>
       <c r="E31" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F31" s="8">
         <v>0</v>
@@ -2160,38 +2166,70 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B32" t="s">
-        <v>80</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
+        <v>39</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>39</v>
       </c>
       <c r="E32" s="8">
+        <v>0</v>
+      </c>
+      <c r="F32" s="8">
+        <v>0</v>
+      </c>
+      <c r="G32" s="11">
+        <v>0</v>
+      </c>
+      <c r="H32" s="11">
+        <v>0</v>
+      </c>
+      <c r="I32" s="11">
+        <v>0</v>
+      </c>
+      <c r="J32" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="8">
         <v>1</v>
       </c>
-      <c r="F32" s="8">
-        <v>0</v>
-      </c>
-      <c r="G32" s="11">
-        <v>0</v>
-      </c>
-      <c r="H32" s="11">
-        <v>0</v>
-      </c>
-      <c r="I32" s="11">
-        <v>0</v>
-      </c>
-      <c r="J32" s="11">
+      <c r="F33" s="8">
+        <v>0</v>
+      </c>
+      <c r="G33" s="11">
+        <v>0</v>
+      </c>
+      <c r="H33" s="11">
+        <v>0</v>
+      </c>
+      <c r="I33" s="11">
+        <v>0</v>
+      </c>
+      <c r="J33" s="11">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J32"/>
+  <autoFilter ref="A1:J33"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
@@ -2231,31 +2269,31 @@
         <v>20</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2266,31 +2304,31 @@
         <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F2" s="17">
         <v>0</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="K2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2301,31 +2339,31 @@
         <v>57</v>
       </c>
       <c r="C3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="17">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="J3" t="s">
         <v>98</v>
       </c>
-      <c r="D3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="17">
-        <v>0</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="H3" t="s">
-        <v>94</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="J3" t="s">
-        <v>96</v>
-      </c>
       <c r="K3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2336,31 +2374,31 @@
         <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F4" s="18">
         <v>8.4</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2371,28 +2409,28 @@
         <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F5" s="17">
         <v>0</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="J5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="K5" t="s">
         <v>14</v>
@@ -2406,28 +2444,28 @@
         <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F6" s="18">
         <v>7.5</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="J6" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="K6" t="s">
         <v>14</v>
@@ -2441,28 +2479,28 @@
         <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F7" s="19">
         <v>5.9</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H7" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="J7" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="K7" t="s">
         <v>14</v>
@@ -2476,28 +2514,28 @@
         <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D8" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F8" s="18">
         <v>7.5</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K8" t="s">
         <v>14</v>
@@ -2511,31 +2549,31 @@
         <v>65</v>
       </c>
       <c r="C9" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F9" s="19">
         <v>4.3</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H9" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="J9" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="K9" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2546,31 +2584,31 @@
         <v>65</v>
       </c>
       <c r="C10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F10" s="20">
         <v>3.1</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="J10" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="K10" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2605,263 +2643,263 @@
   <sheetData>
     <row r="1" ht="25" customHeight="1" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E1" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="16" t="s">
-        <v>87</v>
-      </c>
       <c r="G1" s="9" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C2" s="8">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>95</v>
-      </c>
       <c r="G2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H2" t="s">
         <v>14</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C3" s="8">
         <v>8.4</v>
       </c>
       <c r="D3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="15" t="s">
-        <v>104</v>
-      </c>
       <c r="G3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H3" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C4" s="8">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H4" t="s">
         <v>14</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C5" s="8">
         <v>7.5</v>
       </c>
       <c r="D5" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H5" t="s">
         <v>14</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C6" s="8">
         <v>5.9</v>
       </c>
       <c r="D6" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G6" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H6" t="s">
         <v>14</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C7" s="8">
         <v>7.5</v>
       </c>
       <c r="D7" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G7" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H7" t="s">
         <v>14</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C8" s="8">
         <v>4.3</v>
       </c>
       <c r="D8" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F8" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="F8" s="15" t="s">
-        <v>123</v>
-      </c>
       <c r="G8" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="H8" t="s">
         <v>14</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C9" s="8">
         <v>3.1</v>
       </c>
       <c r="D9" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E9" t="s">
+        <v>132</v>
+      </c>
+      <c r="F9" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="F9" s="15" t="s">
-        <v>128</v>
-      </c>
       <c r="G9" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H9" t="s">
         <v>14</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add : git repo dashboard 추가 modify : 가독성, 차트랜더링
</commit_message>
<xml_diff>
--- a/vulnerability-scanner/output/vulnerability-dashboard.xlsx
+++ b/vulnerability-scanner/output/vulnerability-dashboard.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="141">
   <si>
     <t>🛡️ Vulnerability Scan Summary</t>
   </si>
@@ -22,7 +22,7 @@
     <t>Scan Date:</t>
   </si>
   <si>
-    <t>2025. 12. 22. 오후 1:21:13</t>
+    <t>2025. 12. 23. 오후 5:24:47</t>
   </si>
   <si>
     <t>Scanner Version:</t>
@@ -103,13 +103,160 @@
     <t>🔵 Low</t>
   </si>
   <si>
-    <t>samples/test-project</t>
+    <t>/Users/milk/workspace/cicd</t>
+  </si>
+  <si>
+    <t>cicd</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven-21</t>
+  </si>
+  <si>
+    <t>mobileid</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven</t>
+  </si>
+  <si>
+    <t>boilerplate-maven</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/web-common</t>
+  </si>
+  <si>
+    <t>web-common</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/tour-api</t>
+  </si>
+  <si>
+    <t>tour-api</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/step-hts-server</t>
+  </si>
+  <si>
+    <t>step-hts-server</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/scm-api</t>
+  </si>
+  <si>
+    <t>scm-api</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/partner-gateway</t>
+  </si>
+  <si>
+    <t>partner-gateway</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/order</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/mcp-server</t>
+  </si>
+  <si>
+    <t>mcp-server</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/gateway-util</t>
+  </si>
+  <si>
+    <t>gateway-util</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/gateway-domain</t>
+  </si>
+  <si>
+    <t>gateway-domain</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/channel-gateway</t>
+  </si>
+  <si>
+    <t>channel-gateway</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/auth-api</t>
+  </si>
+  <si>
+    <t>auth-api</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-maven/ai-chatbot</t>
+  </si>
+  <si>
+    <t>ai-chatbot</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/-bmjs/vulnerability-scanner/samples/test-project</t>
   </si>
   <si>
     <t>test-app</t>
   </si>
   <si>
-    <t>unknown</t>
+    <t>/Users/milk/workspace/-bmjs/vulnerability-scanner/samples/repro-tika</t>
+  </si>
+  <si>
+    <t>my-app</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/-bmjs/vulnerability-scanner/samples/java-project</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-mvc</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-mvc/user</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-mvc/local/overrides</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-mvc/gradle/convention</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-mvc/common</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-mvc/api</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-gradle</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-gradle/payment-service</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-gradle/order-service</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-gradle/delivery-service</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-gradle/cve-service</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/boilerplate-gradle/common-events</t>
+  </si>
+  <si>
+    <t>/Users/milk/workspace/-bmjs/vulnerability-scanner/samples/c-project</t>
+  </si>
+  <si>
+    <t>c-project</t>
   </si>
   <si>
     <t>Project Key</t>
@@ -139,6 +286,156 @@
     <t>CWEs</t>
   </si>
   <si>
+    <t>unknown:partner-gateway</t>
+  </si>
+  <si>
+    <t>CVE-2025-48924</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>org.apache.commons:commons-lang3</t>
+  </si>
+  <si>
+    <t>3.13.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncontrolled Recursion vulnerability in Apache Commons Lang.
+This issue affects Apache Commons Lang: Starting with commons-lang:commons-lang 2.0 to 2.6, and, from org.apache.commons:commons-lang3 3.0 before 3.18.0.
+The methods ClassUtils.getClass(...) can throw StackOverflowError on very long inputs. Because an Error is usually not handled by applications and libraries, a 
+StackOverflowError could cause an application to stop.
+Users are recommended to upgrade to version 3.18.0, which fixes the issue.</t>
+  </si>
+  <si>
+    <t>2025-07-11T14:56:58.049Z</t>
+  </si>
+  <si>
+    <t>CWE-674</t>
+  </si>
+  <si>
+    <t>unknown:channel-gateway</t>
+  </si>
+  <si>
+    <t>com.example:my-app</t>
+  </si>
+  <si>
+    <t>CVE-2025-54988</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>org.apache.tika:tika-parser-pdf-module</t>
+  </si>
+  <si>
+    <t>3.2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Critical XXE in Apache Tika (tika-parser-pdf-module) in Apache Tika 1.13 through and including 3.2.1 on all platforms allows an attacker to carry out XML External Entity injection via a crafted XFA file inside of a PDF. An attacker may be able to read sensitive data or trigger malicious requests to internal resources or third-party servers. Note that the tika-parser-pdf-module is used as a dependency in several Tika packages including at least: tika-parsers-standard-modules, tika-parsers-standard-package, tika-app, tika-grpc and tika-server-standard.
+Users are recommended to upgrade to version 3.2.2, which fixes this issue.</t>
+  </si>
+  <si>
+    <t>2025-08-20T20:08:49.481Z</t>
+  </si>
+  <si>
+    <t>CWE-611</t>
+  </si>
+  <si>
+    <t>CVE-2025-41242</t>
+  </si>
+  <si>
+    <t>MEDIUM</t>
+  </si>
+  <si>
+    <t>org.springframework:spring-core</t>
+  </si>
+  <si>
+    <t>5.3.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spring Framework MVC applications can be vulnerable to a “Path Traversal Vulnerability” when deployed on a non-compliant Servlet container.
+An application can be vulnerable when all the following are true:
+  *  the application is deployed as a WAR or with an embedded Servlet container
+  *  the Servlet container  does not reject suspicious sequences https://jakarta.ee/specifications/servlet/6.1/jakarta-servlet-spec-6.1.html#uri-path-canonicalization 
+  *  the application  serves static resources https://docs.spring.io/spring-framework/reference/web/webmvc/mvc-config/static-resources.html#page-title  with Spring resource handling
+We have verified that applications deployed on Apache Tomcat or Eclipse Jetty are not vulnerable, as long as default security features are not disabled in the configuration. Because we cannot check exploits against all Servlet containers and configuration variants, we strongly recommend upgrading your application.</t>
+  </si>
+  <si>
+    <t>2025-08-18T08:47:07.427Z</t>
+  </si>
+  <si>
+    <t>CVE-2025-41249</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Spring Framework annotation detection mechanism may not correctly resolve annotations on methods within type hierarchies with a parameterized super type with unbounded generics. This can be an issue if such annotations are used for authorization decisions.
+Your application may be affected by this if you are using Spring Security's @EnableMethodSecurity feature.
+You are not affected by this if you are not using @EnableMethodSecurity or if you do not use security annotations on methods in generic superclasses or generic interfaces.
+This CVE is published in conjunction with  CVE-2025-41248 https://spring.io/security/cve-2025-41248 .</t>
+  </si>
+  <si>
+    <t>2025-09-16T10:15:34.118Z</t>
+  </si>
+  <si>
+    <t>CVE-2025-41254</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STOMP over WebSocket applications may be vulnerable to a security bypass that allows an attacker to send unauthorized messages.
+Affected Spring Products and VersionsSpring Framework:
+  *  6.2.0 - 6.2.11
+  *  6.1.0 - 6.1.23
+  *  6.0.x - 6.0.29
+  *  5.3.0 - 5.3.45
+  *  Older, unsupported versions are also affected.
+MitigationUsers of affected versions should upgrade to the corresponding fixed version.
+Affected version(s)Fix versionAvailability6.2.x6.2.12OSS6.1.x6.1.24 Commercial https://enterprise.spring.io/ 6.0.xN/A Out of support https://spring.io/projects/spring-framework#support 5.3.x5.3.46 Commercial https://enterprise.spring.io/ No further mitigation steps are necessary.
+CreditThis vulnerability was discovered and responsibly reported by Jannis Kaiser.</t>
+  </si>
+  <si>
+    <t>2025-10-16T14:48:37.350Z</t>
+  </si>
+  <si>
+    <t>CWE-352</t>
+  </si>
+  <si>
+    <t>CVE-2025-22233</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CVE-2024-38820 ensured Locale-independent, lowercase conversion for both the configured disallowedFields patterns and for request parameter names. However, there are still cases where it is possible to bypass the disallowedFields checks.
+Affected Spring Products and Versions
+Spring Framework:
+  *  6.2.0 - 6.2.6
+  *  6.1.0 - 6.1.19
+  *  6.0.0 - 6.0.27
+  *  5.3.0 - 5.3.42
+  *  Older, unsupported versions are also affected
+Mitigation
+Users of affected versions should upgrade to the corresponding fixed version.
+Affected version(s)Fix Version Availability 6.2.x
+ 6.2.7
+OSS6.1.x
+ 6.1.20
+OSS6.0.x
+ 6.0.28
+ Commercial https://enterprise.spring.io/ 5.3.x
+ 5.3.43
+ Commercial https://enterprise.spring.io/ 
+No further mitigation steps are necessary.
+Generally, we recommend using a dedicated model object with properties only for data binding, or using constructor binding since constructor arguments explicitly declare what to bind together with turning off setter binding through the declarativeBinding flag. See the Model Design section in the reference documentation.
+For setting binding, prefer the use of allowedFields (an explicit list) over disallowedFields.
+Credit
+This issue was responsibly reported by the TERASOLUNA Framework Development Team from NTT DATA Group Corporation.</t>
+  </si>
+  <si>
+    <t>2025-05-16T19:14:07.500Z</t>
+  </si>
+  <si>
+    <t>CWE-20</t>
+  </si>
+  <si>
     <t>CVSS Vector</t>
   </si>
   <si>
@@ -149,13 +446,50 @@
   </si>
   <si>
     <t>References</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>https://lists.apache.org/thread/bgv0lpswokgol11tloxnjfzdl7yrc1g1</t>
+  </si>
+  <si>
+    <t>CVSS:3.1/AV:L/AC:L/PR:N/UI:N/S:U/C:H/I:H/A:H</t>
+  </si>
+  <si>
+    <t>https://lists.apache.org/thread/8xn3rqy6kz5b3l1t83kcofkw0w4mmj1w</t>
+  </si>
+  <si>
+    <t>CVSS:3.1/AV:N/AC:H/PR:N/UI:N/S:U/C:H/I:N/A:N</t>
+  </si>
+  <si>
+    <t>http://spring.io/security/cve-2025-41242</t>
+  </si>
+  <si>
+    <t>CVSS:3.1/AV:N/AC:L/PR:N/UI:N/S:U/C:H/I:N/A:N</t>
+  </si>
+  <si>
+    <t>https://spring.io/security/cve-2025-41249</t>
+  </si>
+  <si>
+    <t>CVSS:3.1/AV:N/AC:L/PR:N/UI:R/S:U/C:N/I:L/A:N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://spring.io/security/cve/2025-41254
+https://nvd.nist.gov/vuln-metrics/cvss/v3-calculator?vector=AV:N/AC:L/PR:N/UI:R/S:U/C:N/I:L/A:N&amp;version=3.1</t>
+  </si>
+  <si>
+    <t>CVSS:3.1/AV:N/AC:H/PR:L/UI:N/S:U/C:N/I:L/A:N</t>
+  </si>
+  <si>
+    <t>https://nvd.nist.gov/vuln-metrics/cvss/v3-calculator?vector=AV:N/AC:H/PR:L/UI:N/S:U/C:N/I:L/A:N&amp;version=3.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -198,6 +532,22 @@
     <font>
       <color rgb="FF808080"/>
     </font>
+    <font>
+      <b/>
+      <color rgb="FF8C00"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FFD700"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="4A9EFF"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FFA0A0A0"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -224,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -247,11 +597,32 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -636,7 +1007,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -644,7 +1015,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -652,7 +1023,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -660,7 +1031,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3">
-        <v>1</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -673,7 +1044,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="3">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -681,7 +1052,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -689,7 +1060,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="3">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -713,7 +1084,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -721,7 +1092,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -729,7 +1100,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -746,7 +1117,7 @@
   <sheetPr>
     <tabColor rgb="FF4FACFE"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -810,26 +1181,986 @@
         <v>31</v>
       </c>
       <c r="E2" s="8">
+        <v>6</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0</v>
+      </c>
+      <c r="G2" s="11">
+        <v>0</v>
+      </c>
+      <c r="H2" s="11">
+        <v>0</v>
+      </c>
+      <c r="I2" s="11">
+        <v>0</v>
+      </c>
+      <c r="J2" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="8">
+        <v>3</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0</v>
+      </c>
+      <c r="G3" s="11">
+        <v>0</v>
+      </c>
+      <c r="H3" s="11">
+        <v>0</v>
+      </c>
+      <c r="I3" s="11">
+        <v>0</v>
+      </c>
+      <c r="J3" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11">
+        <v>0</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0</v>
+      </c>
+      <c r="J4" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="8">
+        <v>3</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0</v>
+      </c>
+      <c r="G5" s="11">
+        <v>0</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0</v>
+      </c>
+      <c r="I5" s="11">
+        <v>0</v>
+      </c>
+      <c r="J5" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="8">
+        <v>11</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="11">
+        <v>0</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0</v>
+      </c>
+      <c r="I6" s="11">
+        <v>0</v>
+      </c>
+      <c r="J6" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="8">
+        <v>11</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0</v>
+      </c>
+      <c r="G7" s="11">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0</v>
+      </c>
+      <c r="I7" s="11">
+        <v>0</v>
+      </c>
+      <c r="J7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="8">
+        <v>24</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="11">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0</v>
+      </c>
+      <c r="I8" s="11">
+        <v>0</v>
+      </c>
+      <c r="J8" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="8">
+        <v>18</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0</v>
+      </c>
+      <c r="I9" s="11">
+        <v>0</v>
+      </c>
+      <c r="J9" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="8">
+        <v>6</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0</v>
+      </c>
+      <c r="G10" s="11">
+        <v>0</v>
+      </c>
+      <c r="H10" s="11">
+        <v>0</v>
+      </c>
+      <c r="I10" s="11">
+        <v>0</v>
+      </c>
+      <c r="J10" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="8">
+        <v>5</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0</v>
+      </c>
+      <c r="G11" s="11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="11">
+        <v>0</v>
+      </c>
+      <c r="J11" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="8">
+        <v>11</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0</v>
+      </c>
+      <c r="G12" s="11">
+        <v>0</v>
+      </c>
+      <c r="H12" s="11">
+        <v>0</v>
+      </c>
+      <c r="I12" s="11">
+        <v>0</v>
+      </c>
+      <c r="J12" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="8">
+        <v>3</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0</v>
+      </c>
+      <c r="G13" s="11">
+        <v>0</v>
+      </c>
+      <c r="H13" s="11">
+        <v>0</v>
+      </c>
+      <c r="I13" s="11">
+        <v>0</v>
+      </c>
+      <c r="J13" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="8">
+        <v>17</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0</v>
+      </c>
+      <c r="G14" s="11">
+        <v>0</v>
+      </c>
+      <c r="H14" s="11">
+        <v>0</v>
+      </c>
+      <c r="I14" s="11">
+        <v>0</v>
+      </c>
+      <c r="J14" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="8">
+        <v>18</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0</v>
+      </c>
+      <c r="G15" s="11">
+        <v>0</v>
+      </c>
+      <c r="H15" s="11">
+        <v>0</v>
+      </c>
+      <c r="I15" s="11">
+        <v>0</v>
+      </c>
+      <c r="J15" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="8">
+        <v>11</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0</v>
+      </c>
+      <c r="G16" s="11">
+        <v>0</v>
+      </c>
+      <c r="H16" s="11">
+        <v>0</v>
+      </c>
+      <c r="I16" s="11">
+        <v>0</v>
+      </c>
+      <c r="J16" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="8">
         <v>1</v>
       </c>
-      <c r="F2" s="8">
-        <v>0</v>
-      </c>
-      <c r="G2" s="11">
-        <v>0</v>
-      </c>
-      <c r="H2" s="11">
-        <v>0</v>
-      </c>
-      <c r="I2" s="11">
-        <v>0</v>
-      </c>
-      <c r="J2" s="11">
+      <c r="F17" s="8">
+        <v>0</v>
+      </c>
+      <c r="G17" s="11">
+        <v>0</v>
+      </c>
+      <c r="H17" s="11">
+        <v>0</v>
+      </c>
+      <c r="I17" s="11">
+        <v>0</v>
+      </c>
+      <c r="J17" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="8">
+        <v>2</v>
+      </c>
+      <c r="F18" s="8">
+        <v>0</v>
+      </c>
+      <c r="G18" s="11">
+        <v>0</v>
+      </c>
+      <c r="H18" s="12">
+        <v>1</v>
+      </c>
+      <c r="I18" s="11">
+        <v>0</v>
+      </c>
+      <c r="J18" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="8">
+        <v>1</v>
+      </c>
+      <c r="F19" s="8">
+        <v>0</v>
+      </c>
+      <c r="G19" s="11">
+        <v>0</v>
+      </c>
+      <c r="H19" s="12">
+        <v>1</v>
+      </c>
+      <c r="I19" s="13">
+        <v>2</v>
+      </c>
+      <c r="J19" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="8">
+        <v>0</v>
+      </c>
+      <c r="F20" s="8">
+        <v>0</v>
+      </c>
+      <c r="G20" s="11">
+        <v>0</v>
+      </c>
+      <c r="H20" s="11">
+        <v>0</v>
+      </c>
+      <c r="I20" s="11">
+        <v>0</v>
+      </c>
+      <c r="J20" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="8">
+        <v>2</v>
+      </c>
+      <c r="F21" s="8">
+        <v>0</v>
+      </c>
+      <c r="G21" s="11">
+        <v>0</v>
+      </c>
+      <c r="H21" s="11">
+        <v>0</v>
+      </c>
+      <c r="I21" s="11">
+        <v>0</v>
+      </c>
+      <c r="J21" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="8">
+        <v>0</v>
+      </c>
+      <c r="F22" s="8">
+        <v>0</v>
+      </c>
+      <c r="G22" s="11">
+        <v>0</v>
+      </c>
+      <c r="H22" s="11">
+        <v>0</v>
+      </c>
+      <c r="I22" s="11">
+        <v>0</v>
+      </c>
+      <c r="J22" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="8">
+        <v>0</v>
+      </c>
+      <c r="F23" s="8">
+        <v>0</v>
+      </c>
+      <c r="G23" s="11">
+        <v>0</v>
+      </c>
+      <c r="H23" s="11">
+        <v>0</v>
+      </c>
+      <c r="I23" s="11">
+        <v>0</v>
+      </c>
+      <c r="J23" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="8">
+        <v>1</v>
+      </c>
+      <c r="F24" s="8">
+        <v>0</v>
+      </c>
+      <c r="G24" s="11">
+        <v>0</v>
+      </c>
+      <c r="H24" s="11">
+        <v>0</v>
+      </c>
+      <c r="I24" s="11">
+        <v>0</v>
+      </c>
+      <c r="J24" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="8">
+        <v>3</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0</v>
+      </c>
+      <c r="G25" s="11">
+        <v>0</v>
+      </c>
+      <c r="H25" s="11">
+        <v>0</v>
+      </c>
+      <c r="I25" s="11">
+        <v>0</v>
+      </c>
+      <c r="J25" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" s="8">
+        <v>0</v>
+      </c>
+      <c r="F26" s="8">
+        <v>0</v>
+      </c>
+      <c r="G26" s="11">
+        <v>0</v>
+      </c>
+      <c r="H26" s="11">
+        <v>0</v>
+      </c>
+      <c r="I26" s="11">
+        <v>0</v>
+      </c>
+      <c r="J26" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="8">
+        <v>0</v>
+      </c>
+      <c r="F27" s="8">
+        <v>0</v>
+      </c>
+      <c r="G27" s="11">
+        <v>0</v>
+      </c>
+      <c r="H27" s="11">
+        <v>0</v>
+      </c>
+      <c r="I27" s="11">
+        <v>0</v>
+      </c>
+      <c r="J27" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="8">
+        <v>2</v>
+      </c>
+      <c r="F28" s="8">
+        <v>0</v>
+      </c>
+      <c r="G28" s="11">
+        <v>0</v>
+      </c>
+      <c r="H28" s="11">
+        <v>0</v>
+      </c>
+      <c r="I28" s="11">
+        <v>0</v>
+      </c>
+      <c r="J28" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="8">
+        <v>0</v>
+      </c>
+      <c r="F29" s="8">
+        <v>0</v>
+      </c>
+      <c r="G29" s="11">
+        <v>0</v>
+      </c>
+      <c r="H29" s="11">
+        <v>0</v>
+      </c>
+      <c r="I29" s="11">
+        <v>0</v>
+      </c>
+      <c r="J29" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="8">
+        <v>3</v>
+      </c>
+      <c r="F30" s="8">
+        <v>0</v>
+      </c>
+      <c r="G30" s="11">
+        <v>0</v>
+      </c>
+      <c r="H30" s="11">
+        <v>0</v>
+      </c>
+      <c r="I30" s="11">
+        <v>0</v>
+      </c>
+      <c r="J30" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" s="8">
+        <v>0</v>
+      </c>
+      <c r="F31" s="8">
+        <v>0</v>
+      </c>
+      <c r="G31" s="11">
+        <v>0</v>
+      </c>
+      <c r="H31" s="11">
+        <v>0</v>
+      </c>
+      <c r="I31" s="11">
+        <v>0</v>
+      </c>
+      <c r="J31" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="8">
+        <v>1</v>
+      </c>
+      <c r="F32" s="8">
+        <v>0</v>
+      </c>
+      <c r="G32" s="11">
+        <v>0</v>
+      </c>
+      <c r="H32" s="11">
+        <v>0</v>
+      </c>
+      <c r="I32" s="11">
+        <v>0</v>
+      </c>
+      <c r="J32" s="11">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J2"/>
+  <autoFilter ref="A1:J32"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
@@ -840,7 +2171,7 @@
   <sheetPr>
     <tabColor rgb="FFFF8C00"/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -856,7 +2187,7 @@
     <col min="5" max="6" width="12" style="8" customWidth="1"/>
     <col min="7" max="7" width="40" style="8" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="80" style="12" customWidth="1"/>
+    <col min="9" max="9" width="80" style="15" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
   </cols>
@@ -869,35 +2200,280 @@
         <v>20</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>38</v>
+        <v>86</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>87</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>40</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="17">
+        <v>0</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="J2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="17">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="J3" t="s">
+        <v>96</v>
+      </c>
+      <c r="K3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" s="18">
+        <v>8.4</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="J4" t="s">
+        <v>105</v>
+      </c>
+      <c r="K4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" s="19">
+        <v>5.9</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="J5" t="s">
+        <v>112</v>
+      </c>
+      <c r="K5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="18">
+        <v>7.5</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="J6" t="s">
+        <v>115</v>
+      </c>
+      <c r="K6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" s="19">
+        <v>4.3</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H7" t="s">
+        <v>110</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="J7" t="s">
+        <v>118</v>
+      </c>
+      <c r="K7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" s="20">
+        <v>3.1</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="J8" t="s">
+        <v>123</v>
+      </c>
+      <c r="K8" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K1"/>
+  <autoFilter ref="A1:K8"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
@@ -908,7 +2484,7 @@
   <sheetPr>
     <tabColor rgb="FFFFD700"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -921,42 +2497,216 @@
     <col min="2" max="3" width="12" style="8" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="80" style="12" customWidth="1"/>
+    <col min="6" max="6" width="80" style="15" customWidth="1"/>
     <col min="7" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="60" style="12" customWidth="1"/>
+    <col min="9" max="9" width="60" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>38</v>
+        <v>89</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>87</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>42</v>
+        <v>126</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>44</v>
+        <v>127</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="8">
+        <v>8.4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="G3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="8">
+        <v>5.9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="G5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="8">
+        <v>4.3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E6" t="s">
+        <v>119</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="G6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="8">
+        <v>3.1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="G7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1"/>
+  <autoFilter ref="A1:I7"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>